<commit_message>
handler for timer5 done, keypad library must be fix
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S4IOT\Desktop\STMCube_Courses\Bare-Metal\Proyecto_personal\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\STMCube_Courses\Bare-Metal\Proyecto_personal\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107F175D-9D93-434E-B114-DD168045C8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5CEBBD-314B-4D4E-96D0-3B2982F6FBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11175" yWindow="960" windowWidth="15375" windowHeight="7875" xr2:uid="{F68614E3-D65F-42D8-8E49-5E7634DEE3C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F68614E3-D65F-42D8-8E49-5E7634DEE3C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -443,6 +443,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,9 +490,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,32 +807,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FA1A01-ED58-41EB-B003-64EB3BEB0F97}">
   <dimension ref="B1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" zoomScale="110" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="I16" sqref="G16:I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
@@ -846,7 +846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="18">
         <v>0</v>
       </c>
@@ -866,7 +866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="18">
         <v>1</v>
       </c>
@@ -885,7 +885,7 @@
       <c r="J4" s="5"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="18">
         <v>4</v>
       </c>
@@ -903,7 +903,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="18">
         <v>5</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="18">
         <v>6</v>
       </c>
@@ -927,7 +927,7 @@
       </c>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
         <v>7</v>
       </c>
@@ -942,7 +942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
         <v>8</v>
       </c>
@@ -957,7 +957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="18">
         <v>9</v>
       </c>
@@ -969,7 +969,7 @@
       </c>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="18">
         <v>10</v>
       </c>
@@ -981,7 +981,7 @@
       </c>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="18">
         <v>11</v>
       </c>
@@ -993,7 +993,7 @@
       </c>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="18">
         <v>12</v>
       </c>
@@ -1004,13 +1004,13 @@
         <v>10</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="18">
         <v>15</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="18"/>
       <c r="C15" s="18">
         <v>14</v>
@@ -1050,7 +1050,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="19"/>
       <c r="C16" s="19">
         <v>15</v>
@@ -1069,7 +1069,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="13"/>
       <c r="G17" s="1" t="s">
         <v>25</v>
@@ -1081,7 +1081,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G18" s="1" t="s">
         <v>26</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G19" s="1" t="s">
         <v>27</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1114,125 +1114,125 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
         <v>1</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="20">
         <v>2</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="20">
         <v>3</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="10">
         <v>4</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="10">
         <v>5</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="34"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="33"/>
+      <c r="D26" s="35"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <v>6</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="34"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="33"/>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="10">
         <v>7</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="34"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="33"/>
+      <c r="D28" s="35"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="10">
         <v>8</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="34"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="35"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="10">
         <v>9</v>
       </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="34"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="34"/>
+      <c r="D30" s="35"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="10">
         <v>10</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="34"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="34"/>
+      <c r="D31" s="35"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>11</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="34"/>
+      <c r="D32" s="35"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="10">
         <v>12</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="20">
         <v>13</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="20">
         <v>14</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="10">
         <v>15</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
         <v>1</v>
       </c>
@@ -1243,123 +1243,123 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="11">
         <v>0</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
         <v>2</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" s="22">
         <v>3</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" s="11">
         <v>4</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
         <v>5</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" s="11">
         <v>6</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="11"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <v>7</v>
       </c>
       <c r="C47" s="11"/>
-      <c r="D47" s="35" t="s">
+      <c r="D47" s="36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
         <v>8</v>
       </c>
       <c r="C48" s="11"/>
-      <c r="D48" s="36"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="37"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="11">
         <v>9</v>
       </c>
       <c r="C49" s="11"/>
-      <c r="D49" s="36"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="37"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="11">
         <v>10</v>
       </c>
       <c r="C50" s="11"/>
-      <c r="D50" s="36"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="37"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="22">
         <v>11</v>
       </c>
       <c r="C51" s="23"/>
-      <c r="D51" s="36"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="37"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
         <v>12</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="C52" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D52" s="36"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D52" s="37"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="11">
         <v>13</v>
       </c>
-      <c r="C53" s="39"/>
-      <c r="D53" s="36"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="40"/>
+      <c r="D53" s="37"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
         <v>14</v>
       </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="36"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="40"/>
+      <c r="D54" s="37"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
         <v>15</v>
       </c>
-      <c r="C55" s="40"/>
-      <c r="D55" s="37"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="41"/>
+      <c r="D55" s="38"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
         <v>0</v>
       </c>
@@ -1373,77 +1373,77 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="11">
         <v>0</v>
       </c>
-      <c r="C59" s="29" t="s">
+      <c r="C59" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E59" s="31" t="s">
+      <c r="E59" s="32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="11">
         <v>1</v>
       </c>
-      <c r="C60" s="29"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="31"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C60" s="30"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="32"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="11">
         <v>2</v>
       </c>
-      <c r="C61" s="29"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="31"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C61" s="30"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="32"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="11">
         <v>3</v>
       </c>
-      <c r="C62" s="29"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="31"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C62" s="30"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="32"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="11">
         <v>4</v>
       </c>
-      <c r="C63" s="29"/>
+      <c r="C63" s="30"/>
       <c r="D63" s="24"/>
-      <c r="E63" s="31"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="32"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="11">
         <v>5</v>
       </c>
-      <c r="C64" s="29"/>
+      <c r="C64" s="30"/>
       <c r="D64" s="25"/>
-      <c r="E64" s="31"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="32"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="11">
         <v>6</v>
       </c>
-      <c r="C65" s="29"/>
+      <c r="C65" s="30"/>
       <c r="D65" s="25"/>
-      <c r="E65" s="31"/>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="32"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="11">
         <v>7</v>
       </c>
-      <c r="C66" s="29"/>
+      <c r="C66" s="30"/>
       <c r="D66" s="25"/>
-      <c r="E66" s="31"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="32"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="11">
         <v>8</v>
       </c>
@@ -1451,7 +1451,7 @@
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="11">
         <v>9</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="11">
         <v>10</v>
       </c>
@@ -1467,7 +1467,7 @@
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="11">
         <v>11</v>
       </c>
@@ -1475,7 +1475,7 @@
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="11">
         <v>12</v>
       </c>
@@ -1483,7 +1483,7 @@
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="11">
         <v>13</v>
       </c>
@@ -1491,7 +1491,7 @@
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="22">
         <v>14</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="D73" s="22"/>
       <c r="E73" s="22"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="22">
         <v>15</v>
       </c>
@@ -1507,12 +1507,12 @@
       <c r="D74" s="22"/>
       <c r="E74" s="22"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="11">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
library keypad 4x4 done, test OpC and OpA
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\STMCube_Courses\Bare-Metal\Proyecto_personal\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5CEBBD-314B-4D4E-96D0-3B2982F6FBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BF2583-54C2-4789-ADD4-3F0FFEF21739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F68614E3-D65F-42D8-8E49-5E7634DEE3C2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Port C</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>4x4 teclado</t>
-  </si>
-  <si>
-    <t>motor</t>
   </si>
   <si>
     <t>Puerto A</t>
@@ -141,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +199,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -388,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -434,9 +437,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -461,9 +461,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -473,15 +470,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,6 +478,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -807,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FA1A01-ED58-41EB-B003-64EB3BEB0F97}">
   <dimension ref="B1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="I16" sqref="G16:I16"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="149" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,12 +831,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
@@ -863,7 +872,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
@@ -939,7 +948,7 @@
       </c>
       <c r="E8" s="18"/>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
@@ -954,7 +963,7 @@
       </c>
       <c r="E9" s="18"/>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
@@ -1004,11 +1013,11 @@
         <v>10</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="G13" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
+      <c r="G13" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="18">
@@ -1022,13 +1031,13 @@
       </c>
       <c r="E14" s="18"/>
       <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -1041,13 +1050,13 @@
       </c>
       <c r="E15" s="18"/>
       <c r="G15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="1">
         <v>16</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1060,58 +1069,58 @@
       </c>
       <c r="E16" s="19"/>
       <c r="G16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H16" s="1">
         <v>32</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="13"/>
       <c r="G17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="1">
         <v>16</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="1">
         <v>16</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="1">
         <v>16</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
@@ -1146,10 +1155,10 @@
       <c r="B25" s="10">
         <v>4</v>
       </c>
-      <c r="C25" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="35" t="s">
+      <c r="C25" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="33" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1157,52 +1166,52 @@
       <c r="B26" s="10">
         <v>5</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="35"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="33"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <v>6</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="35"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="33"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="10">
         <v>7</v>
       </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="35"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="33"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="10">
         <v>8</v>
       </c>
-      <c r="C29" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="35"/>
+      <c r="C29" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="33"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="10">
         <v>9</v>
       </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="35"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="33"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="10">
         <v>10</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="35"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>11</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="35"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="10">
@@ -1237,10 +1246,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
@@ -1297,9 +1306,7 @@
         <v>7</v>
       </c>
       <c r="C47" s="11"/>
-      <c r="D47" s="36" t="s">
-        <v>6</v>
-      </c>
+      <c r="D47" s="37"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
@@ -1323,18 +1330,18 @@
       <c r="D50" s="37"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="22">
+      <c r="B51" s="38">
         <v>11</v>
       </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="37"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="40"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
         <v>12</v>
       </c>
-      <c r="C52" s="39" t="s">
-        <v>7</v>
+      <c r="C52" s="34" t="s">
+        <v>14</v>
       </c>
       <c r="D52" s="37"/>
     </row>
@@ -1342,106 +1349,106 @@
       <c r="B53" s="11">
         <v>13</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="35"/>
       <c r="D53" s="37"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
         <v>14</v>
       </c>
-      <c r="C54" s="40"/>
+      <c r="C54" s="35"/>
       <c r="D54" s="37"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
         <v>15</v>
       </c>
-      <c r="C55" s="41"/>
-      <c r="D55" s="38"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="37"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="11">
         <v>0</v>
       </c>
-      <c r="C59" s="30" t="s">
+      <c r="C59" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D59" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E59" s="32" t="s">
-        <v>6</v>
-      </c>
+      <c r="E59" s="37"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="11">
         <v>1</v>
       </c>
-      <c r="C60" s="30"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="32"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="37"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="11">
         <v>2</v>
       </c>
-      <c r="C61" s="30"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="37"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="11">
         <v>3</v>
       </c>
-      <c r="C62" s="30"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="32"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="37"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="11">
         <v>4</v>
       </c>
-      <c r="C63" s="30"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="32"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="37"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="11">
         <v>5</v>
       </c>
-      <c r="C64" s="30"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="32"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="43"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="11">
         <v>6</v>
       </c>
-      <c r="C65" s="30"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="32"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="41" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="11">
         <v>7</v>
       </c>
-      <c r="C66" s="30"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="32"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="41"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="11">
@@ -1449,7 +1456,7 @@
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
+      <c r="E67" s="41"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="11">
@@ -1457,7 +1464,7 @@
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
+      <c r="E68" s="41"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="11">
@@ -1465,7 +1472,7 @@
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
+      <c r="E69" s="41"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="11">
@@ -1473,7 +1480,7 @@
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
+      <c r="E70" s="41"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="11">
@@ -1481,7 +1488,7 @@
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
+      <c r="E71" s="41"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="11">
@@ -1489,7 +1496,7 @@
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
+      <c r="E72" s="42"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="22">
@@ -1518,17 +1525,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C59:C66"/>
     <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E66"/>
     <mergeCell ref="C25:C28"/>
     <mergeCell ref="C29:C32"/>
     <mergeCell ref="D25:D32"/>
-    <mergeCell ref="D47:D55"/>
     <mergeCell ref="C52:C55"/>
+    <mergeCell ref="E65:E72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
start with lcd library
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\STMCube_Courses\Bare-Metal\Proyecto_personal\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2BF2583-54C2-4789-ADD4-3F0FFEF21739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24832EC2-D758-4CD4-A2D8-1F5BAEBF356C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F68614E3-D65F-42D8-8E49-5E7634DEE3C2}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Port C</t>
   </si>
@@ -123,6 +121,12 @@
   </si>
   <si>
     <t>up</t>
+  </si>
+  <si>
+    <t>LCD</t>
+  </si>
+  <si>
+    <t>funcion 4</t>
   </si>
 </sst>
 </file>
@@ -138,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +209,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -391,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -443,6 +459,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -479,26 +507,32 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -816,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FA1A01-ED58-41EB-B003-64EB3BEB0F97}">
   <dimension ref="B1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="149" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65:E72"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="149" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -831,12 +865,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
@@ -1013,11 +1047,11 @@
         <v>10</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="18">
@@ -1155,10 +1189,10 @@
       <c r="B25" s="10">
         <v>4</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="37" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1166,52 +1200,52 @@
       <c r="B26" s="10">
         <v>5</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="33"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="37"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <v>6</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="33"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="37"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="10">
         <v>7</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="33"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="37"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="10">
         <v>8</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="33"/>
+      <c r="D29" s="37"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="10">
         <v>9</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="10">
         <v>10</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="33"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="37"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>11</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="33"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="37"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="10">
@@ -1285,88 +1319,90 @@
         <v>4</v>
       </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
+      <c r="D44" s="43" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
         <v>5</v>
       </c>
       <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
+      <c r="D45" s="44"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" s="11">
         <v>6</v>
       </c>
       <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
+      <c r="D46" s="44"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <v>7</v>
       </c>
       <c r="C47" s="11"/>
-      <c r="D47" s="37"/>
+      <c r="D47" s="44"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
         <v>8</v>
       </c>
       <c r="C48" s="11"/>
-      <c r="D48" s="37"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D48" s="44"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" s="11">
         <v>9</v>
       </c>
       <c r="C49" s="11"/>
-      <c r="D49" s="37"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D49" s="44"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="11">
         <v>10</v>
       </c>
       <c r="C50" s="11"/>
-      <c r="D50" s="37"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="38">
+      <c r="D50" s="45"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="25">
         <v>11</v>
       </c>
-      <c r="C51" s="39"/>
-      <c r="D51" s="40"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C51" s="26"/>
+      <c r="D51" s="27"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
         <v>12</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="C52" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="37"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D52" s="24"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" s="11">
         <v>13</v>
       </c>
-      <c r="C53" s="35"/>
-      <c r="D53" s="37"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C53" s="39"/>
+      <c r="D53" s="24"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
         <v>14</v>
       </c>
-      <c r="C54" s="35"/>
-      <c r="D54" s="37"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C54" s="39"/>
+      <c r="D54" s="24"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
         <v>15</v>
       </c>
-      <c r="C55" s="36"/>
-      <c r="D55" s="37"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C55" s="40"/>
+      <c r="D55" s="24"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
         <v>0</v>
       </c>
@@ -1379,153 +1415,174 @@
       <c r="E58" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F58" s="46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" s="11">
         <v>0</v>
       </c>
-      <c r="C59" s="29" t="s">
+      <c r="C59" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E59" s="37"/>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E59" s="24"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" s="11">
         <v>1</v>
       </c>
-      <c r="C60" s="29"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="37"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C60" s="33"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="11">
         <v>2</v>
       </c>
-      <c r="C61" s="29"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="37"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C61" s="33"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="11">
         <v>3</v>
       </c>
-      <c r="C62" s="29"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="37"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C62" s="33"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" s="11">
         <v>4</v>
       </c>
-      <c r="C63" s="29"/>
+      <c r="C63" s="33"/>
       <c r="D63" s="23"/>
-      <c r="E63" s="37"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E63" s="24"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" s="11">
         <v>5</v>
       </c>
-      <c r="C64" s="29"/>
+      <c r="C64" s="33"/>
       <c r="D64" s="24"/>
-      <c r="E64" s="43"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E64" s="28"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="11">
         <v>6</v>
       </c>
-      <c r="C65" s="29"/>
+      <c r="C65" s="33"/>
       <c r="D65" s="24"/>
       <c r="E65" s="41" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="11">
         <v>7</v>
       </c>
-      <c r="C66" s="29"/>
+      <c r="C66" s="33"/>
       <c r="D66" s="24"/>
       <c r="E66" s="41"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F66" s="47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="11">
         <v>8</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="41"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F67" s="48"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="11">
         <v>9</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
       <c r="E68" s="41"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F68" s="48"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="11">
         <v>10</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
       <c r="E69" s="41"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F69" s="48"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="11">
         <v>11</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
       <c r="E70" s="41"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F70" s="48"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="11">
         <v>12</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="41"/>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F71" s="48"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="11">
         <v>13</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="42"/>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F72" s="49"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="22">
         <v>14</v>
       </c>
       <c r="C73" s="22"/>
       <c r="D73" s="22"/>
       <c r="E73" s="22"/>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="22">
         <v>15</v>
       </c>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
       <c r="E74" s="22"/>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F74" s="1"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="11">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C59:C66"/>
@@ -1535,6 +1592,8 @@
     <mergeCell ref="D25:D32"/>
     <mergeCell ref="C52:C55"/>
     <mergeCell ref="E65:E72"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="F66:F72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
lcd_init and set_command function done, ready to test
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\STMCube_Courses\Bare-Metal\Proyecto_personal\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24832EC2-D758-4CD4-A2D8-1F5BAEBF356C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3220EA3C-467C-40EF-A2D6-25C879C6CDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F68614E3-D65F-42D8-8E49-5E7634DEE3C2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>Port C</t>
   </si>
@@ -127,6 +127,27 @@
   </si>
   <si>
     <t>funcion 4</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D4</t>
   </si>
 </sst>
 </file>
@@ -407,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -513,25 +534,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -850,13 +859,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FA1A01-ED58-41EB-B003-64EB3BEB0F97}">
   <dimension ref="B1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="149" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="149" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
     <col min="8" max="8" width="15.109375" customWidth="1"/>
     <col min="9" max="9" width="16.44140625" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" customWidth="1"/>
@@ -1247,132 +1257,159 @@
       <c r="C32" s="36"/>
       <c r="D32" s="37"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="10">
         <v>12</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="20">
         <v>13</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="20">
         <v>14</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="10">
         <v>15</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E39" s="43"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="11">
         <v>0</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
         <v>2</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="22">
         <v>3</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E43" s="22"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="11">
         <v>4</v>
       </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="43" t="s">
+      <c r="D44" s="44" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E44" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
         <v>5</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="44"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E45" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="11">
         <v>6</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="44"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E46" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <v>7</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="44"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E47" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
         <v>8</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="44"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E48" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="11">
         <v>9</v>
       </c>
       <c r="C49" s="11"/>
       <c r="D49" s="44"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E49" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" s="11">
         <v>10</v>
       </c>
       <c r="C50" s="11"/>
-      <c r="D50" s="45"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D50" s="44"/>
+      <c r="E50" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="25">
         <v>11</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="27"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E51" s="27"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
         <v>12</v>
       </c>
@@ -1380,29 +1417,33 @@
         <v>14</v>
       </c>
       <c r="D52" s="24"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" s="11">
         <v>13</v>
       </c>
       <c r="C53" s="39"/>
       <c r="D53" s="24"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
         <v>14</v>
       </c>
       <c r="C54" s="39"/>
       <c r="D54" s="24"/>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
         <v>15</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="24"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E55" s="1"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
         <v>0</v>
       </c>
@@ -1415,11 +1456,12 @@
       <c r="E58" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F58" s="46" t="s">
+      <c r="F58" s="43" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G58" s="43"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59" s="11">
         <v>0</v>
       </c>
@@ -1431,8 +1473,9 @@
       </c>
       <c r="E59" s="24"/>
       <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60" s="11">
         <v>1</v>
       </c>
@@ -1440,8 +1483,9 @@
       <c r="D60" s="34"/>
       <c r="E60" s="24"/>
       <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" s="11">
         <v>2</v>
       </c>
@@ -1449,8 +1493,9 @@
       <c r="D61" s="34"/>
       <c r="E61" s="24"/>
       <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" s="11">
         <v>3</v>
       </c>
@@ -1458,8 +1503,9 @@
       <c r="D62" s="34"/>
       <c r="E62" s="24"/>
       <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" s="11">
         <v>4</v>
       </c>
@@ -1467,8 +1513,9 @@
       <c r="D63" s="23"/>
       <c r="E63" s="24"/>
       <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64" s="11">
         <v>5</v>
       </c>
@@ -1476,8 +1523,9 @@
       <c r="D64" s="24"/>
       <c r="E64" s="28"/>
       <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" s="11">
         <v>6</v>
       </c>
@@ -1487,73 +1535,95 @@
         <v>6</v>
       </c>
       <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" s="11">
         <v>7</v>
       </c>
       <c r="C66" s="33"/>
       <c r="D66" s="24"/>
       <c r="E66" s="41"/>
-      <c r="F66" s="47" t="s">
+      <c r="F66" s="45" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G66" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" s="11">
         <v>8</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="41"/>
-      <c r="F67" s="48"/>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F67" s="45"/>
+      <c r="G67" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" s="11">
         <v>9</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
       <c r="E68" s="41"/>
-      <c r="F68" s="48"/>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F68" s="45"/>
+      <c r="G68" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" s="11">
         <v>10</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
       <c r="E69" s="41"/>
-      <c r="F69" s="48"/>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F69" s="45"/>
+      <c r="G69" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" s="11">
         <v>11</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
       <c r="E70" s="41"/>
-      <c r="F70" s="48"/>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F70" s="45"/>
+      <c r="G70" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71" s="11">
         <v>12</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="41"/>
-      <c r="F71" s="48"/>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F71" s="45"/>
+      <c r="G71" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72" s="11">
         <v>13</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="42"/>
-      <c r="F72" s="49"/>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F72" s="45"/>
+      <c r="G72" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B73" s="22">
         <v>14</v>
       </c>
@@ -1561,8 +1631,9 @@
       <c r="D73" s="22"/>
       <c r="E73" s="22"/>
       <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74" s="22">
         <v>15</v>
       </c>
@@ -1570,19 +1641,20 @@
       <c r="D74" s="22"/>
       <c r="E74" s="22"/>
       <c r="F74" s="1"/>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G74" s="1"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78" s="11">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C59:C66"/>
@@ -1594,6 +1666,8 @@
     <mergeCell ref="E65:E72"/>
     <mergeCell ref="D44:D50"/>
     <mergeCell ref="F66:F72"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F58:G58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
lcd library done, including print and using keypad
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\STMCube_Courses\Bare-Metal\Proyecto_personal\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3220EA3C-467C-40EF-A2D6-25C879C6CDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2539F88A-E9AB-4FFD-8AC9-E15F2A3B6514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F68614E3-D65F-42D8-8E49-5E7634DEE3C2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>Port C</t>
   </si>
@@ -148,13 +148,43 @@
   </si>
   <si>
     <t>D4</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>button b1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,8 +192,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,8 +280,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA162D0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4343"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -424,11 +480,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -492,6 +585,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,21 +630,56 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF4343"/>
+      <color rgb="FFFF6600"/>
+      <color rgb="FFA162D0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -857,35 +988,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FA1A01-ED58-41EB-B003-64EB3BEB0F97}">
-  <dimension ref="B1:K78"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="149" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
-    <col min="11" max="11" width="8.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="12"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I1" s="12"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
@@ -898,8 +1031,9 @@
       <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F2" s="48"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="18">
         <v>0</v>
       </c>
@@ -912,14 +1046,15 @@
       <c r="E3" s="18">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="48"/>
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="18">
         <v>1</v>
       </c>
@@ -930,15 +1065,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="18"/>
-      <c r="G4" t="s">
+      <c r="F4" s="48"/>
+      <c r="H4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="18">
         <v>4</v>
       </c>
@@ -949,14 +1085,15 @@
         <v>2</v>
       </c>
       <c r="E5" s="18"/>
-      <c r="G5" t="s">
+      <c r="F5" s="48"/>
+      <c r="H5" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="18">
         <v>5</v>
       </c>
@@ -967,8 +1104,9 @@
         <v>3</v>
       </c>
       <c r="E6" s="18"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F6" s="48"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="18">
         <v>6</v>
       </c>
@@ -979,8 +1117,9 @@
         <v>4</v>
       </c>
       <c r="E7" s="18"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F7" s="48"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
         <v>7</v>
       </c>
@@ -991,11 +1130,12 @@
         <v>5</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="G8" t="s">
+      <c r="F8" s="48"/>
+      <c r="H8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
         <v>8</v>
       </c>
@@ -1006,11 +1146,12 @@
         <v>6</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="G9" t="s">
+      <c r="F9" s="48"/>
+      <c r="H9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="18">
         <v>9</v>
       </c>
@@ -1021,8 +1162,9 @@
         <v>7</v>
       </c>
       <c r="E10" s="18"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F10" s="48"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="18">
         <v>10</v>
       </c>
@@ -1033,8 +1175,9 @@
         <v>8</v>
       </c>
       <c r="E11" s="18"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F11" s="48"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="18">
         <v>11</v>
       </c>
@@ -1045,8 +1188,9 @@
         <v>9</v>
       </c>
       <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F12" s="48"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="18">
         <v>12</v>
       </c>
@@ -1057,13 +1201,14 @@
         <v>10</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="G13" s="29" t="s">
+      <c r="F13" s="48"/>
+      <c r="H13" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="18">
         <v>15</v>
       </c>
@@ -1074,17 +1219,18 @@
         <v>11</v>
       </c>
       <c r="E14" s="18"/>
-      <c r="G14" s="1" t="s">
+      <c r="F14" s="48"/>
+      <c r="H14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="18"/>
       <c r="C15" s="18">
         <v>14</v>
@@ -1093,17 +1239,18 @@
         <v>12</v>
       </c>
       <c r="E15" s="18"/>
-      <c r="G15" s="1" t="s">
+      <c r="F15" s="48"/>
+      <c r="H15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>16</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="19"/>
       <c r="C16" s="19">
         <v>15</v>
@@ -1112,224 +1259,283 @@
         <v>13</v>
       </c>
       <c r="E16" s="19"/>
-      <c r="G16" s="1" t="s">
+      <c r="F16" s="48"/>
+      <c r="H16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>32</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B17" s="13"/>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>16</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G18" s="1" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>16</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G19" s="1" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>16</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E20" s="30"/>
+      <c r="F20" s="49"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E21" s="1"/>
+      <c r="F21" s="50"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
         <v>1</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E22" s="1"/>
+      <c r="F22" s="50"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" s="20">
         <v>2</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E23" s="21"/>
+      <c r="F23" s="54"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24" s="20">
         <v>3</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E24" s="21"/>
+      <c r="F24" s="55"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25" s="10">
         <v>4</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="38" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E25" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="54"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
       <c r="B26" s="10">
         <v>5</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="37"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C26" s="36"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="54"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <v>6</v>
       </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="37"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C27" s="36"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="54"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" s="10">
         <v>7</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="37"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C28" s="36"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="54"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29" s="10">
         <v>8</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="37"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D29" s="38"/>
+      <c r="E29" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="54"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B30" s="10">
         <v>9</v>
       </c>
-      <c r="C30" s="36"/>
-      <c r="D30" s="37"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C30" s="37"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="54"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31" s="10">
         <v>10</v>
       </c>
-      <c r="C31" s="36"/>
-      <c r="D31" s="37"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C31" s="37"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="54"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>11</v>
       </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="37"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="54"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="10">
         <v>12</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="1"/>
+      <c r="F33" s="54"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="20">
         <v>13</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="21"/>
+      <c r="F34" s="54"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="20">
         <v>14</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="21"/>
+      <c r="F35" s="54"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="10">
         <v>15</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="1"/>
+      <c r="F36" s="54"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="43" t="s">
+      <c r="D39" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="43"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="46"/>
+      <c r="F39" s="48"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="11">
         <v>0</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F40" s="50"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F41" s="50"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
         <v>2</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F42" s="50"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="22">
         <v>3</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F43" s="56"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="11">
         <v>4</v>
       </c>
@@ -1337,113 +1543,125 @@
       <c r="D44" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="60" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F44" s="54"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
         <v>5</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="44"/>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="60" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F45" s="54"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="11">
         <v>6</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="44"/>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="60" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F46" s="54"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <v>7</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="44"/>
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="60" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F47" s="54"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
         <v>8</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="44"/>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="60" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F48" s="54"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" s="11">
         <v>9</v>
       </c>
       <c r="C49" s="11"/>
       <c r="D49" s="44"/>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="60" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F49" s="54"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="11">
         <v>10</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="44"/>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="60" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F50" s="54"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="25">
         <v>11</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F51" s="57"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
         <v>12</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="C52" s="39" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="24"/>
       <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F52" s="50"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B53" s="11">
         <v>13</v>
       </c>
-      <c r="C53" s="39"/>
+      <c r="C53" s="40"/>
       <c r="D53" s="24"/>
       <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F53" s="50"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
         <v>14</v>
       </c>
-      <c r="C54" s="39"/>
+      <c r="C54" s="40"/>
       <c r="D54" s="24"/>
       <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F54" s="50"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
         <v>15</v>
       </c>
-      <c r="C55" s="40"/>
+      <c r="C55" s="41"/>
       <c r="D55" s="24"/>
       <c r="E55" s="1"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F55" s="50"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
         <v>0</v>
       </c>
@@ -1453,209 +1671,245 @@
       <c r="D58" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="E58" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F58" s="43" t="s">
+      <c r="F58" s="52"/>
+      <c r="G58" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="G58" s="43"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H58" s="46"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B59" s="11">
         <v>0</v>
       </c>
-      <c r="C59" s="33" t="s">
+      <c r="C59" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="35" t="s">
         <v>14</v>
       </c>
       <c r="E59" s="24"/>
-      <c r="F59" s="1"/>
+      <c r="F59" s="24"/>
       <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B60" s="11">
         <v>1</v>
       </c>
-      <c r="C60" s="33"/>
-      <c r="D60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="35"/>
       <c r="E60" s="24"/>
-      <c r="F60" s="1"/>
+      <c r="F60" s="24"/>
       <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H60" s="1"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B61" s="11">
         <v>2</v>
       </c>
-      <c r="C61" s="33"/>
-      <c r="D61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="35"/>
       <c r="E61" s="24"/>
-      <c r="F61" s="1"/>
+      <c r="F61" s="24"/>
       <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B62" s="11">
         <v>3</v>
       </c>
-      <c r="C62" s="33"/>
-      <c r="D62" s="34"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="35"/>
       <c r="E62" s="24"/>
-      <c r="F62" s="1"/>
+      <c r="F62" s="24"/>
       <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B63" s="11">
         <v>4</v>
       </c>
-      <c r="C63" s="33"/>
+      <c r="C63" s="34"/>
       <c r="D63" s="23"/>
       <c r="E63" s="24"/>
-      <c r="F63" s="1"/>
+      <c r="F63" s="24"/>
       <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B64" s="11">
         <v>5</v>
       </c>
-      <c r="C64" s="33"/>
+      <c r="C64" s="34"/>
       <c r="D64" s="24"/>
       <c r="E64" s="28"/>
-      <c r="F64" s="1"/>
+      <c r="F64" s="28"/>
       <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B65" s="11">
         <v>6</v>
       </c>
-      <c r="C65" s="33"/>
+      <c r="C65" s="34"/>
       <c r="D65" s="24"/>
-      <c r="E65" s="41" t="s">
+      <c r="E65" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="F65" s="1"/>
+      <c r="F65" s="53" t="s">
+        <v>39</v>
+      </c>
       <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B66" s="11">
         <v>7</v>
       </c>
-      <c r="C66" s="33"/>
+      <c r="C66" s="34"/>
       <c r="D66" s="24"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="45" t="s">
+      <c r="E66" s="42"/>
+      <c r="F66" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="H66" s="58" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B67" s="11">
         <v>8</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="41"/>
-      <c r="F67" s="45"/>
-      <c r="G67" s="1" t="s">
+      <c r="E67" s="42"/>
+      <c r="F67" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="G67" s="45"/>
+      <c r="H67" s="58" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B68" s="11">
         <v>9</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
-      <c r="E68" s="41"/>
-      <c r="F68" s="45"/>
-      <c r="G68" s="1" t="s">
+      <c r="E68" s="42"/>
+      <c r="F68" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="G68" s="45"/>
+      <c r="H68" s="58" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B69" s="11">
         <v>10</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
-      <c r="E69" s="41"/>
-      <c r="F69" s="45"/>
-      <c r="G69" s="1" t="s">
+      <c r="E69" s="42"/>
+      <c r="F69" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="G69" s="45"/>
+      <c r="H69" s="58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B70" s="11">
         <v>11</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
-      <c r="E70" s="41"/>
-      <c r="F70" s="45"/>
-      <c r="G70" s="1" t="s">
+      <c r="E70" s="42"/>
+      <c r="F70" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="G70" s="45"/>
+      <c r="H70" s="58" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B71" s="11">
         <v>12</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
-      <c r="E71" s="41"/>
-      <c r="F71" s="45"/>
-      <c r="G71" s="1" t="s">
+      <c r="E71" s="42"/>
+      <c r="F71" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="G71" s="45"/>
+      <c r="H71" s="58" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B72" s="11">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>47</v>
+      </c>
+      <c r="B72" s="29">
         <v>13</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
-      <c r="E72" s="42"/>
-      <c r="F72" s="45"/>
-      <c r="G72" s="1" t="s">
+      <c r="E72" s="43"/>
+      <c r="F72" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="G72" s="45"/>
+      <c r="H72" s="58" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B73" s="22">
         <v>14</v>
       </c>
       <c r="C73" s="22"/>
       <c r="D73" s="22"/>
       <c r="E73" s="22"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F73" s="22"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B74" s="22">
         <v>15</v>
       </c>
       <c r="C74" s="22"/>
       <c r="D74" s="22"/>
       <c r="E74" s="22"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F74" s="22"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B77" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B78" s="11">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="G13:I13"/>
+  <mergeCells count="15">
+    <mergeCell ref="H13:J13"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C59:C66"/>
     <mergeCell ref="D59:D62"/>
@@ -1665,10 +1919,13 @@
     <mergeCell ref="C52:C55"/>
     <mergeCell ref="E65:E72"/>
     <mergeCell ref="D44:D50"/>
-    <mergeCell ref="F66:F72"/>
+    <mergeCell ref="G66:G72"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="E58:F58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add functions to star or stop timers, modification of pins to lcd and kaypad
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\STMCube_Courses\Bare-Metal\Proyecto_personal\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2539F88A-E9AB-4FFD-8AC9-E15F2A3B6514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F68614E3-D65F-42D8-8E49-5E7634DEE3C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>Port C</t>
   </si>
@@ -178,12 +177,15 @@
   </si>
   <si>
     <t>button b1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pendientes por pasar lcd y teclado un pin arriba en fisico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -582,61 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -649,12 +597,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -667,6 +609,76 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,10 +999,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FA1A01-ED58-41EB-B003-64EB3BEB0F97}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="145" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
@@ -1007,13 +1019,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="29"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
@@ -1031,7 +1043,7 @@
       <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="48"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="18">
@@ -1046,7 +1058,7 @@
       <c r="E3" s="18">
         <v>2</v>
       </c>
-      <c r="F3" s="48"/>
+      <c r="F3" s="30"/>
       <c r="H3" t="s">
         <v>4</v>
       </c>
@@ -1065,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="18"/>
-      <c r="F4" s="48"/>
+      <c r="F4" s="30"/>
       <c r="H4" t="s">
         <v>5</v>
       </c>
@@ -1085,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="18"/>
-      <c r="F5" s="48"/>
+      <c r="F5" s="30"/>
       <c r="H5" t="s">
         <v>6</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="18"/>
-      <c r="F6" s="48"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="18">
@@ -1117,7 +1129,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="18"/>
-      <c r="F7" s="48"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
@@ -1130,7 +1142,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="48"/>
+      <c r="F8" s="30"/>
       <c r="H8" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1158,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="48"/>
+      <c r="F9" s="30"/>
       <c r="H9" t="s">
         <v>18</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="18"/>
-      <c r="F10" s="48"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="18">
@@ -1175,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="48"/>
+      <c r="F11" s="30"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="18">
@@ -1188,7 +1200,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="18"/>
-      <c r="F12" s="48"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="18">
@@ -1201,12 +1213,12 @@
         <v>10</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="F13" s="48"/>
-      <c r="H13" s="30" t="s">
+      <c r="F13" s="30"/>
+      <c r="H13" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="18">
@@ -1219,7 +1231,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="18"/>
-      <c r="F14" s="48"/>
+      <c r="F14" s="30"/>
       <c r="H14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1239,7 +1251,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="18"/>
-      <c r="F15" s="48"/>
+      <c r="F15" s="30"/>
       <c r="H15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="19"/>
-      <c r="F16" s="48"/>
+      <c r="F16" s="30"/>
       <c r="H16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1311,11 +1323,11 @@
       <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="49"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
@@ -1324,7 +1336,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="50"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
@@ -1333,7 +1345,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="50"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B23" s="20">
@@ -1342,7 +1354,7 @@
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
-      <c r="F23" s="54"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B24" s="20">
@@ -1351,22 +1363,22 @@
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="55"/>
+      <c r="F24" s="35"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B25" s="10">
         <v>4</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="54"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1375,80 +1387,80 @@
       <c r="B26" s="10">
         <v>5</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="59" t="s">
+      <c r="C26" s="53"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="54"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <v>6</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="59" t="s">
+      <c r="C27" s="53"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="54"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B28" s="10">
         <v>7</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="59" t="s">
+      <c r="C28" s="53"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="54"/>
+      <c r="F28" s="34"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B29" s="10">
         <v>8</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="38"/>
-      <c r="E29" s="59" t="s">
+      <c r="D29" s="55"/>
+      <c r="E29" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="54"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B30" s="10">
         <v>9</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="59" t="s">
+      <c r="C30" s="54"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="54"/>
+      <c r="F30" s="34"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B31" s="10">
         <v>10</v>
       </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="59" t="s">
+      <c r="C31" s="54"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="F31" s="54"/>
+      <c r="F31" s="34"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>11</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="59" t="s">
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="54"/>
+      <c r="F32" s="34"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="10">
@@ -1457,7 +1469,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="54"/>
+      <c r="F33" s="34"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="20">
@@ -1466,7 +1478,7 @@
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="54"/>
+      <c r="F34" s="34"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="20">
@@ -1475,7 +1487,7 @@
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
       <c r="E35" s="21"/>
-      <c r="F35" s="54"/>
+      <c r="F35" s="34"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="10">
@@ -1484,7 +1496,7 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="54"/>
+      <c r="F36" s="34"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
@@ -1493,11 +1505,11 @@
       <c r="C39" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="46" t="s">
+      <c r="D39" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="46"/>
-      <c r="F39" s="48"/>
+      <c r="E39" s="60"/>
+      <c r="F39" s="30"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="11">
@@ -1506,7 +1518,7 @@
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="50"/>
+      <c r="F40" s="32"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="11">
@@ -1515,7 +1527,7 @@
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="50"/>
+      <c r="F41" s="32"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
@@ -1524,7 +1536,7 @@
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="50"/>
+      <c r="F42" s="32"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="22">
@@ -1533,86 +1545,86 @@
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="56"/>
+      <c r="F43" s="36"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="11">
         <v>4</v>
       </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="60" t="s">
+      <c r="E44" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="F44" s="54"/>
+      <c r="F44" s="34"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
         <v>5</v>
       </c>
       <c r="C45" s="11"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="60" t="s">
+      <c r="D45" s="59"/>
+      <c r="E45" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="54"/>
+      <c r="F45" s="34"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="11">
         <v>6</v>
       </c>
       <c r="C46" s="11"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="60" t="s">
+      <c r="D46" s="59"/>
+      <c r="E46" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="54"/>
+      <c r="F46" s="34"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <v>7</v>
       </c>
       <c r="C47" s="11"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="60" t="s">
+      <c r="D47" s="59"/>
+      <c r="E47" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="F47" s="54"/>
+      <c r="F47" s="34"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
         <v>8</v>
       </c>
       <c r="C48" s="11"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="60" t="s">
+      <c r="D48" s="59"/>
+      <c r="E48" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F48" s="54"/>
+      <c r="F48" s="34"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" s="11">
         <v>9</v>
       </c>
       <c r="C49" s="11"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="60" t="s">
+      <c r="D49" s="59"/>
+      <c r="E49" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F49" s="54"/>
+      <c r="F49" s="34"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="11">
         <v>10</v>
       </c>
       <c r="C50" s="11"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="60" t="s">
+      <c r="D50" s="59"/>
+      <c r="E50" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="F50" s="54"/>
+      <c r="F50" s="34"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B51" s="25">
@@ -1621,45 +1633,45 @@
       <c r="C51" s="26"/>
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
-      <c r="F51" s="57"/>
+      <c r="F51" s="37"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
         <v>12</v>
       </c>
-      <c r="C52" s="39" t="s">
+      <c r="C52" s="56" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="24"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="50"/>
+      <c r="F52" s="32"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B53" s="11">
         <v>13</v>
       </c>
-      <c r="C53" s="40"/>
+      <c r="C53" s="57"/>
       <c r="D53" s="24"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="50"/>
+      <c r="F53" s="32"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
         <v>14</v>
       </c>
-      <c r="C54" s="40"/>
+      <c r="C54" s="57"/>
       <c r="D54" s="24"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="50"/>
+      <c r="F54" s="32"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
         <v>15</v>
       </c>
-      <c r="C55" s="41"/>
+      <c r="C55" s="58"/>
       <c r="D55" s="24"/>
       <c r="E55" s="1"/>
-      <c r="F55" s="50"/>
+      <c r="F55" s="32"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
@@ -1671,23 +1683,23 @@
       <c r="D58" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="51" t="s">
+      <c r="E58" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F58" s="52"/>
-      <c r="G58" s="46" t="s">
+      <c r="F58" s="62"/>
+      <c r="G58" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="H58" s="46"/>
+      <c r="H58" s="60"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B59" s="11">
         <v>0</v>
       </c>
-      <c r="C59" s="34" t="s">
+      <c r="C59" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="35" t="s">
+      <c r="D59" s="52" t="s">
         <v>14</v>
       </c>
       <c r="E59" s="24"/>
@@ -1699,8 +1711,8 @@
       <c r="B60" s="11">
         <v>1</v>
       </c>
-      <c r="C60" s="34"/>
-      <c r="D60" s="35"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="52"/>
       <c r="E60" s="24"/>
       <c r="F60" s="24"/>
       <c r="G60" s="1"/>
@@ -1710,8 +1722,8 @@
       <c r="B61" s="11">
         <v>2</v>
       </c>
-      <c r="C61" s="34"/>
-      <c r="D61" s="35"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="52"/>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
       <c r="G61" s="1"/>
@@ -1721,8 +1733,8 @@
       <c r="B62" s="11">
         <v>3</v>
       </c>
-      <c r="C62" s="34"/>
-      <c r="D62" s="35"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="52"/>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
       <c r="G62" s="1"/>
@@ -1732,7 +1744,7 @@
       <c r="B63" s="11">
         <v>4</v>
       </c>
-      <c r="C63" s="34"/>
+      <c r="C63" s="51"/>
       <c r="D63" s="23"/>
       <c r="E63" s="24"/>
       <c r="F63" s="24"/>
@@ -1743,139 +1755,142 @@
       <c r="B64" s="11">
         <v>5</v>
       </c>
-      <c r="C64" s="34"/>
+      <c r="C64" s="51"/>
       <c r="D64" s="24"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
+      <c r="E64" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="33" t="s">
+        <v>39</v>
+      </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B65" s="11">
         <v>6</v>
       </c>
-      <c r="C65" s="34"/>
+      <c r="C65" s="51"/>
       <c r="D65" s="24"/>
-      <c r="E65" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="F65" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E65" s="64"/>
+      <c r="F65" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="G65" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="H65" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="I65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B66" s="11">
         <v>7</v>
       </c>
-      <c r="C66" s="34"/>
+      <c r="C66" s="51"/>
       <c r="D66" s="24"/>
-      <c r="E66" s="42"/>
-      <c r="F66" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="G66" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="H66" s="58" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E66" s="64"/>
+      <c r="F66" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G66" s="45"/>
+      <c r="H66" s="38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B67" s="11">
         <v>8</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="42"/>
-      <c r="F67" s="53" t="s">
-        <v>41</v>
+      <c r="E67" s="64"/>
+      <c r="F67" s="33" t="s">
+        <v>42</v>
       </c>
       <c r="G67" s="45"/>
-      <c r="H67" s="58" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H67" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B68" s="11">
         <v>9</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
-      <c r="E68" s="42"/>
-      <c r="F68" s="53" t="s">
-        <v>42</v>
+      <c r="E68" s="64"/>
+      <c r="F68" s="33" t="s">
+        <v>43</v>
       </c>
       <c r="G68" s="45"/>
-      <c r="H68" s="58" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H68" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B69" s="11">
         <v>10</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
-      <c r="E69" s="42"/>
-      <c r="F69" s="53" t="s">
-        <v>43</v>
+      <c r="E69" s="64"/>
+      <c r="F69" s="33" t="s">
+        <v>44</v>
       </c>
       <c r="G69" s="45"/>
-      <c r="H69" s="58" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H69" s="38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B70" s="11">
         <v>11</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
-      <c r="E70" s="42"/>
-      <c r="F70" s="53" t="s">
-        <v>44</v>
+      <c r="E70" s="64"/>
+      <c r="F70" s="33" t="s">
+        <v>45</v>
       </c>
       <c r="G70" s="45"/>
-      <c r="H70" s="58" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H70" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B71" s="11">
         <v>12</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
-      <c r="E71" s="42"/>
-      <c r="F71" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="G71" s="45"/>
-      <c r="H71" s="58" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E71" s="64"/>
+      <c r="F71" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="G71" s="46"/>
+      <c r="H71" s="38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>47</v>
       </c>
-      <c r="B72" s="29">
+      <c r="B72" s="28">
         <v>13</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="G72" s="45"/>
-      <c r="H72" s="58" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E72" s="41"/>
+      <c r="F72" s="42"/>
+      <c r="G72" s="43"/>
+      <c r="H72" s="42"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B73" s="22">
         <v>14</v>
       </c>
@@ -1886,7 +1901,7 @@
       <c r="G73" s="21"/>
       <c r="H73" s="21"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B74" s="22">
         <v>15</v>
       </c>
@@ -1897,18 +1912,19 @@
       <c r="G74" s="21"/>
       <c r="H74" s="21"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B77" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B78" s="11">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="G65:G71"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C59:C66"/>
@@ -1917,13 +1933,12 @@
     <mergeCell ref="C29:C32"/>
     <mergeCell ref="D25:D32"/>
     <mergeCell ref="C52:C55"/>
-    <mergeCell ref="E65:E72"/>
     <mergeCell ref="D44:D50"/>
-    <mergeCell ref="G66:G72"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="G58:H58"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E64:E71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
start with ADC librari
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="97">
   <si>
     <t>Port C</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Pines y puertos disponibles</t>
   </si>
   <si>
-    <t>checar que pin era el malo del puerto B</t>
-  </si>
-  <si>
     <t xml:space="preserve">se descarto el puerto B para funcion 8 bits debido a que en el pin B4 no responde a la secuencia </t>
   </si>
   <si>
@@ -179,7 +176,154 @@
     <t>button b1</t>
   </si>
   <si>
-    <t xml:space="preserve"> Pendientes por pasar lcd y teclado un pin arriba en fisico</t>
+    <t>ADC channel</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>channel 0</t>
+  </si>
+  <si>
+    <t>channel 1</t>
+  </si>
+  <si>
+    <t>channel 2</t>
+  </si>
+  <si>
+    <t>channel 3</t>
+  </si>
+  <si>
+    <t>channel 4</t>
+  </si>
+  <si>
+    <t>channel 5</t>
+  </si>
+  <si>
+    <t>channel 6</t>
+  </si>
+  <si>
+    <t>channel 7</t>
+  </si>
+  <si>
+    <t>channel 8</t>
+  </si>
+  <si>
+    <t>channel 9</t>
+  </si>
+  <si>
+    <t>channel 10</t>
+  </si>
+  <si>
+    <t>channel 11</t>
+  </si>
+  <si>
+    <t>channel 12</t>
+  </si>
+  <si>
+    <t>channel 13</t>
+  </si>
+  <si>
+    <t>channel 14</t>
+  </si>
+  <si>
+    <t>channel 15</t>
+  </si>
+  <si>
+    <t>GPIO_C0</t>
+  </si>
+  <si>
+    <t>GPIO_C1</t>
+  </si>
+  <si>
+    <t>GPIO_C2</t>
+  </si>
+  <si>
+    <t>GPIO_C3</t>
+  </si>
+  <si>
+    <t>GPIO_C4</t>
+  </si>
+  <si>
+    <t>GPIO_C5</t>
+  </si>
+  <si>
+    <t>GPIO_A0</t>
+  </si>
+  <si>
+    <t>GPIO_A1</t>
+  </si>
+  <si>
+    <t>GPIO_A2</t>
+  </si>
+  <si>
+    <t>GPIO_A3</t>
+  </si>
+  <si>
+    <t>GPIO_A4</t>
+  </si>
+  <si>
+    <t>GPIO_A5</t>
+  </si>
+  <si>
+    <t>GPIO_A6</t>
+  </si>
+  <si>
+    <t>GPIO_A7</t>
+  </si>
+  <si>
+    <t>GPIO_B0</t>
+  </si>
+  <si>
+    <t>GPIO_B1</t>
+  </si>
+  <si>
+    <t>Function 3</t>
+  </si>
+  <si>
+    <t>Function 5</t>
+  </si>
+  <si>
+    <t>ADC_CHN1</t>
+  </si>
+  <si>
+    <t>ADC_CHN0</t>
+  </si>
+  <si>
+    <t>ADC_CHN4</t>
+  </si>
+  <si>
+    <t>ADC_CHN5</t>
+  </si>
+  <si>
+    <t>ADC_CHN6</t>
+  </si>
+  <si>
+    <t>ADC_CHN7</t>
+  </si>
+  <si>
+    <t>ADC_CHN8</t>
+  </si>
+  <si>
+    <t>ADC_CHN9</t>
+  </si>
+  <si>
+    <t>ADC_CHN10</t>
+  </si>
+  <si>
+    <t>ADC_CHN11</t>
+  </si>
+  <si>
+    <t>ADC_CHN12</t>
+  </si>
+  <si>
+    <t>ADC_CHN13</t>
+  </si>
+  <si>
+    <t>ADC_CHN14</t>
+  </si>
+  <si>
+    <t>ADC_CHN15</t>
   </si>
 </sst>
 </file>
@@ -203,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,6 +444,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -523,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -584,9 +740,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,18 +769,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -679,6 +841,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L78"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="145" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="145" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,19 +1193,19 @@
     <col min="13" max="13" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="29"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="28"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
@@ -1043,9 +1218,10 @@
       <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="30"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="18">
         <v>0</v>
       </c>
@@ -1058,15 +1234,14 @@
       <c r="E3" s="18">
         <v>2</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="H3" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="18">
         <v>1</v>
       </c>
@@ -1077,16 +1252,17 @@
         <v>1</v>
       </c>
       <c r="E4" s="18"/>
-      <c r="F4" s="30"/>
-      <c r="H4" t="s">
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="I4" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="18">
         <v>4</v>
       </c>
@@ -1097,15 +1273,16 @@
         <v>2</v>
       </c>
       <c r="E5" s="18"/>
-      <c r="F5" s="30"/>
-      <c r="H5" t="s">
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="I5" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="18">
         <v>5</v>
       </c>
@@ -1116,9 +1293,10 @@
         <v>3</v>
       </c>
       <c r="E6" s="18"/>
-      <c r="F6" s="30"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="18">
         <v>6</v>
       </c>
@@ -1129,9 +1307,10 @@
         <v>4</v>
       </c>
       <c r="E7" s="18"/>
-      <c r="F7" s="30"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
         <v>7</v>
       </c>
@@ -1142,12 +1321,13 @@
         <v>5</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="30"/>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
         <v>8</v>
       </c>
@@ -1158,12 +1338,13 @@
         <v>6</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="30"/>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="18">
         <v>9</v>
       </c>
@@ -1174,9 +1355,10 @@
         <v>7</v>
       </c>
       <c r="E10" s="18"/>
-      <c r="F10" s="30"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="18">
         <v>10</v>
       </c>
@@ -1187,9 +1369,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="30"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="18">
         <v>11</v>
       </c>
@@ -1200,9 +1383,10 @@
         <v>9</v>
       </c>
       <c r="E12" s="18"/>
-      <c r="F12" s="30"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="18">
         <v>12</v>
       </c>
@@ -1213,14 +1397,15 @@
         <v>10</v>
       </c>
       <c r="E13" s="18"/>
-      <c r="F13" s="30"/>
-      <c r="H13" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="47"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="I13" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="18">
         <v>15</v>
       </c>
@@ -1231,18 +1416,19 @@
         <v>11</v>
       </c>
       <c r="E14" s="18"/>
-      <c r="F14" s="30"/>
-      <c r="H14" s="1" t="s">
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="18"/>
       <c r="C15" s="18">
         <v>14</v>
@@ -1251,18 +1437,19 @@
         <v>12</v>
       </c>
       <c r="E15" s="18"/>
-      <c r="F15" s="30"/>
-      <c r="H15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="I15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="1">
         <v>16</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="19"/>
       <c r="C16" s="19">
         <v>15</v>
@@ -1271,409 +1458,569 @@
         <v>13</v>
       </c>
       <c r="E16" s="19"/>
-      <c r="F16" s="30"/>
-      <c r="H16" s="1" t="s">
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="I16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="1">
+        <v>32</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="13"/>
+      <c r="I17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="1">
-        <v>32</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="J17" s="1">
+        <v>16</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="1">
+        <v>16</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="13"/>
-      <c r="H17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17" s="1">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="1">
         <v>16</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="1">
-        <v>16</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="1">
-        <v>16</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="47"/>
-      <c r="F20" s="31"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E20" s="49"/>
+      <c r="F20" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="32"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F21" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="31"/>
+      <c r="I21" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" s="45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
         <v>1</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="32"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F22" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="31"/>
+      <c r="I22" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B23" s="20">
         <v>2</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
-      <c r="F23" s="34"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F23" s="21"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="J23" s="45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B24" s="20">
         <v>3</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
-      <c r="F24" s="35"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F24" s="21"/>
+      <c r="G24" s="34"/>
+      <c r="I24" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25" s="10">
         <v>4</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="73" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="33"/>
+      <c r="I25" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="J25" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="69">
+        <v>5</v>
+      </c>
+      <c r="C26" s="55"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="34"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="10">
-        <v>5</v>
-      </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="34"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F26" s="73" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="33"/>
+      <c r="I26" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <v>6</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="F27" s="34"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C27" s="55"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="33"/>
+      <c r="I27" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27" s="45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B28" s="10">
         <v>7</v>
       </c>
-      <c r="C28" s="53"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="34"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C28" s="55"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="73" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="33"/>
+      <c r="I28" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" s="45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B29" s="10">
         <v>8</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="55"/>
-      <c r="E29" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="34"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D29" s="57"/>
+      <c r="E29" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="41"/>
+      <c r="G29" s="33"/>
+      <c r="I29" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="J29" s="45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B30" s="10">
         <v>9</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="34"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="41"/>
+      <c r="G30" s="33"/>
+      <c r="I30" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="J30" s="45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B31" s="10">
         <v>10</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" s="34"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="70"/>
+      <c r="G31" s="33"/>
+      <c r="I31" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="J31" s="45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>11</v>
       </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="F32" s="34"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="41"/>
+      <c r="G32" s="33"/>
+      <c r="I32" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" s="45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="10">
         <v>12</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="34"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="41"/>
+      <c r="G33" s="33"/>
+      <c r="I33" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="J33" s="45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="20">
         <v>13</v>
       </c>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="34"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F34" s="21"/>
+      <c r="G34" s="33"/>
+      <c r="I34" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="J34" s="45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="20">
         <v>14</v>
       </c>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
       <c r="E35" s="21"/>
-      <c r="F35" s="34"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="21"/>
+      <c r="G35" s="33"/>
+      <c r="I35" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="J35" s="45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" s="10">
         <v>15</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="34"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="41"/>
+      <c r="G36" s="33"/>
+      <c r="I36" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="I37" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="J37" s="45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="60"/>
-      <c r="F39" s="30"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E39" s="62"/>
+      <c r="F39" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" s="29"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" s="11">
         <v>0</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="32"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F40" s="73" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="31"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="32"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F41" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="G41" s="31"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
         <v>2</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="32"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F42" s="1"/>
+      <c r="G42" s="31"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" s="22">
         <v>3</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="36"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F43" s="22"/>
+      <c r="G43" s="35"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="11">
         <v>4</v>
       </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="59" t="s">
-        <v>29</v>
-      </c>
-      <c r="E44" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44" s="34"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D44" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" s="41"/>
+      <c r="G44" s="33"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
         <v>5</v>
       </c>
       <c r="C45" s="11"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="34"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D45" s="61"/>
+      <c r="E45" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="41"/>
+      <c r="G45" s="33"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="11">
         <v>6</v>
       </c>
       <c r="C46" s="11"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" s="34"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D46" s="61"/>
+      <c r="E46" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="41"/>
+      <c r="G46" s="33"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <v>7</v>
       </c>
       <c r="C47" s="11"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="F47" s="34"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D47" s="61"/>
+      <c r="E47" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="41"/>
+      <c r="G47" s="33"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
         <v>8</v>
       </c>
       <c r="C48" s="11"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="F48" s="34"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D48" s="61"/>
+      <c r="E48" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F48" s="41"/>
+      <c r="G48" s="33"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" s="11">
         <v>9</v>
       </c>
       <c r="C49" s="11"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="F49" s="34"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D49" s="61"/>
+      <c r="E49" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="F49" s="41"/>
+      <c r="G49" s="33"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="11">
         <v>10</v>
       </c>
       <c r="C50" s="11"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F50" s="34"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D50" s="61"/>
+      <c r="E50" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" s="41"/>
+      <c r="G50" s="33"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="25">
         <v>11</v>
       </c>
       <c r="C51" s="26"/>
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
-      <c r="F51" s="37"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F51" s="27"/>
+      <c r="G51" s="36"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
         <v>12</v>
       </c>
-      <c r="C52" s="56" t="s">
+      <c r="C52" s="58" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="24"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="32"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F52" s="1"/>
+      <c r="G52" s="31"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="11">
         <v>13</v>
       </c>
-      <c r="C53" s="57"/>
+      <c r="C53" s="59"/>
       <c r="D53" s="24"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="32"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F53" s="1"/>
+      <c r="G53" s="31"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
         <v>14</v>
       </c>
-      <c r="C54" s="57"/>
+      <c r="C54" s="59"/>
       <c r="D54" s="24"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="32"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F54" s="1"/>
+      <c r="G54" s="31"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
         <v>15</v>
       </c>
-      <c r="C55" s="58"/>
+      <c r="C55" s="60"/>
       <c r="D55" s="24"/>
       <c r="E55" s="1"/>
-      <c r="F55" s="32"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F55" s="1"/>
+      <c r="G55" s="31"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
         <v>0</v>
       </c>
@@ -1683,123 +2030,143 @@
       <c r="D58" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="61" t="s">
+      <c r="E58" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="F58" s="62"/>
-      <c r="G58" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="H58" s="60"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F58" s="64"/>
+      <c r="G58" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="H58" s="62"/>
+      <c r="I58" s="67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" s="11">
         <v>0</v>
       </c>
-      <c r="C59" s="51" t="s">
+      <c r="C59" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="52" t="s">
+      <c r="D59" s="54" t="s">
         <v>14</v>
       </c>
       <c r="E59" s="24"/>
       <c r="F59" s="24"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I59" s="73" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" s="11">
         <v>1</v>
       </c>
-      <c r="C60" s="51"/>
-      <c r="D60" s="52"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="54"/>
       <c r="E60" s="24"/>
       <c r="F60" s="24"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I60" s="73" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="11">
         <v>2</v>
       </c>
-      <c r="C61" s="51"/>
-      <c r="D61" s="52"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="54"/>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I61" s="73" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" s="11">
         <v>3</v>
       </c>
-      <c r="C62" s="51"/>
-      <c r="D62" s="52"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="54"/>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I62" s="73" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" s="11">
         <v>4</v>
       </c>
-      <c r="C63" s="51"/>
+      <c r="C63" s="53"/>
       <c r="D63" s="23"/>
       <c r="E63" s="24"/>
       <c r="F63" s="24"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I63" s="73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" s="11">
         <v>5</v>
       </c>
-      <c r="C64" s="51"/>
+      <c r="C64" s="53"/>
       <c r="D64" s="24"/>
-      <c r="E64" s="63" t="s">
+      <c r="E64" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="F64" s="33" t="s">
-        <v>39</v>
+      <c r="F64" s="32" t="s">
+        <v>38</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
+      <c r="I64" s="73" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B65" s="11">
         <v>6</v>
       </c>
-      <c r="C65" s="51"/>
+      <c r="C65" s="53"/>
       <c r="D65" s="24"/>
-      <c r="E65" s="64"/>
-      <c r="F65" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G65" s="44" t="s">
-        <v>29</v>
-      </c>
-      <c r="H65" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="I65" t="s">
-        <v>48</v>
-      </c>
+      <c r="E65" s="66"/>
+      <c r="F65" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G65" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B66" s="11">
         <v>7</v>
       </c>
-      <c r="C66" s="51"/>
+      <c r="C66" s="53"/>
       <c r="D66" s="24"/>
-      <c r="E66" s="64"/>
-      <c r="F66" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="G66" s="45"/>
-      <c r="H66" s="38" t="s">
-        <v>32</v>
-      </c>
+      <c r="E66" s="66"/>
+      <c r="F66" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" s="47"/>
+      <c r="H66" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B67" s="11">
@@ -1807,14 +2174,15 @@
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="64"/>
-      <c r="F67" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="G67" s="45"/>
-      <c r="H67" s="38" t="s">
-        <v>33</v>
-      </c>
+      <c r="E67" s="66"/>
+      <c r="F67" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="G67" s="47"/>
+      <c r="H67" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="I67" s="1"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B68" s="11">
@@ -1822,14 +2190,15 @@
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="G68" s="45"/>
-      <c r="H68" s="38" t="s">
-        <v>37</v>
-      </c>
+      <c r="E68" s="66"/>
+      <c r="F68" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G68" s="47"/>
+      <c r="H68" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="I68" s="1"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B69" s="11">
@@ -1837,14 +2206,15 @@
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
-      <c r="E69" s="64"/>
-      <c r="F69" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="G69" s="45"/>
-      <c r="H69" s="38" t="s">
-        <v>36</v>
-      </c>
+      <c r="E69" s="66"/>
+      <c r="F69" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="G69" s="47"/>
+      <c r="H69" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="I69" s="1"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B70" s="11">
@@ -1852,14 +2222,15 @@
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
-      <c r="E70" s="64"/>
-      <c r="F70" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="G70" s="45"/>
-      <c r="H70" s="38" t="s">
-        <v>35</v>
-      </c>
+      <c r="E70" s="66"/>
+      <c r="F70" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G70" s="47"/>
+      <c r="H70" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" s="1"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B71" s="11">
@@ -1867,28 +2238,30 @@
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
-      <c r="E71" s="64"/>
-      <c r="F71" s="33" t="s">
+      <c r="E71" s="66"/>
+      <c r="F71" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G71" s="48"/>
+      <c r="H71" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G71" s="46"/>
-      <c r="H71" s="38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>47</v>
-      </c>
-      <c r="B72" s="28">
+      <c r="B72" s="44">
         <v>13</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
-      <c r="E72" s="41"/>
-      <c r="F72" s="42"/>
-      <c r="G72" s="43"/>
-      <c r="H72" s="42"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="42"/>
+      <c r="H72" s="41"/>
+      <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B73" s="22">
@@ -1900,6 +2273,7 @@
       <c r="F73" s="22"/>
       <c r="G73" s="21"/>
       <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B74" s="22">
@@ -1911,6 +2285,7 @@
       <c r="F74" s="22"/>
       <c r="G74" s="21"/>
       <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B77" s="11" t="s">
@@ -1925,7 +2300,7 @@
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="G65:G71"/>
-    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="I13:K13"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C59:C66"/>
     <mergeCell ref="D59:D62"/>

</xml_diff>

<commit_message>
start with PWM developmen libraries, test TIM3
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23148" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="149">
   <si>
     <t>Port C</t>
   </si>
@@ -324,13 +324,171 @@
   </si>
   <si>
     <t>ADC_CHN15</t>
+  </si>
+  <si>
+    <t>No global interrupt</t>
+  </si>
+  <si>
+    <t>Yes global interrupt</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Pin_A0</t>
+  </si>
+  <si>
+    <t>Pin_A1</t>
+  </si>
+  <si>
+    <t>Pin_A2</t>
+  </si>
+  <si>
+    <t>TIM5_CH1</t>
+  </si>
+  <si>
+    <t>TIM5_CH2</t>
+  </si>
+  <si>
+    <t>TIM5_CH3,
+TIM9_CH1</t>
+  </si>
+  <si>
+    <t>Pin_A3</t>
+  </si>
+  <si>
+    <t>TIM5_CH4,
+TIM9_CH2</t>
+  </si>
+  <si>
+    <t>Pin_A6</t>
+  </si>
+  <si>
+    <t>TIM3_CH1</t>
+  </si>
+  <si>
+    <t>Pin_A7</t>
+  </si>
+  <si>
+    <t>TIM3_CH2</t>
+  </si>
+  <si>
+    <t>Pin_B0</t>
+  </si>
+  <si>
+    <t>TIM3_CH3</t>
+  </si>
+  <si>
+    <t>Pin_B1</t>
+  </si>
+  <si>
+    <t>TIM3_CH4</t>
+  </si>
+  <si>
+    <t>Pin_D12</t>
+  </si>
+  <si>
+    <t>TIM4_CH1</t>
+  </si>
+  <si>
+    <t>Pin_D13</t>
+  </si>
+  <si>
+    <t>TIM4_CH2</t>
+  </si>
+  <si>
+    <t>Pin_D14</t>
+  </si>
+  <si>
+    <t>TIM4_CH3</t>
+  </si>
+  <si>
+    <t>Pin_D15</t>
+  </si>
+  <si>
+    <t>TIM4_CH4</t>
+  </si>
+  <si>
+    <t>Pin_C6</t>
+  </si>
+  <si>
+    <t>Pin_C7</t>
+  </si>
+  <si>
+    <t>Pin_C8</t>
+  </si>
+  <si>
+    <t>Pin_C9</t>
+  </si>
+  <si>
+    <t>Pin_B4</t>
+  </si>
+  <si>
+    <t>Pin_B5</t>
+  </si>
+  <si>
+    <t>Pin_B6</t>
+  </si>
+  <si>
+    <t>Pin_B7</t>
+  </si>
+  <si>
+    <t>Pin_B8</t>
+  </si>
+  <si>
+    <t>Pin_B9</t>
+  </si>
+  <si>
+    <t>probar si funciona encender algo con estos pines</t>
+  </si>
+  <si>
+    <t>PWM_TIM5_CH1</t>
+  </si>
+  <si>
+    <t>PWM_TIM5_CH2</t>
+  </si>
+  <si>
+    <t>PWM_TIM3_CH3</t>
+  </si>
+  <si>
+    <t>PWM_TIM3_CH4</t>
+  </si>
+  <si>
+    <t>PWM_TIM3_CH1</t>
+  </si>
+  <si>
+    <t>PWM_TIM3_CH2</t>
+  </si>
+  <si>
+    <t>PWM_TIM4_CH1</t>
+  </si>
+  <si>
+    <t>PWM_TIM4_CH2</t>
+  </si>
+  <si>
+    <t>PWM_TIM4_CH3</t>
+  </si>
+  <si>
+    <t>PWM_TIM4_CH4</t>
+  </si>
+  <si>
+    <t>ALT funtion</t>
+  </si>
+  <si>
+    <t>AF2</t>
+  </si>
+  <si>
+    <t>AF2,AF3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +504,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u val="double"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,8 +622,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -675,11 +859,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -778,67 +971,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -854,6 +987,117 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1175,37 +1419,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M78"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="145" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="153" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
     <col min="8" max="8" width="19.88671875" customWidth="1"/>
     <col min="9" max="9" width="15.109375" customWidth="1"/>
     <col min="10" max="10" width="16.44140625" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="13" max="14" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="50" t="s">
+    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
       <c r="F1" s="28"/>
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
@@ -1221,7 +1466,7 @@
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="18">
         <v>0</v>
       </c>
@@ -1241,7 +1486,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="18">
         <v>1</v>
       </c>
@@ -1261,8 +1506,9 @@
       <c r="K4" s="4"/>
       <c r="L4" s="5"/>
       <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="18">
         <v>4</v>
       </c>
@@ -1282,7 +1528,7 @@
       <c r="K5" s="8"/>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="18">
         <v>5</v>
       </c>
@@ -1296,7 +1542,7 @@
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="18">
         <v>6</v>
       </c>
@@ -1310,7 +1556,7 @@
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
         <v>7</v>
       </c>
@@ -1327,7 +1573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
         <v>8</v>
       </c>
@@ -1344,7 +1590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="18">
         <v>9</v>
       </c>
@@ -1358,7 +1604,7 @@
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="18">
         <v>10</v>
       </c>
@@ -1372,7 +1618,7 @@
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="18">
         <v>11</v>
       </c>
@@ -1386,7 +1632,7 @@
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="18">
         <v>12</v>
       </c>
@@ -1399,13 +1645,13 @@
       <c r="E13" s="18"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
-      <c r="I13" s="49" t="s">
+      <c r="I13" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="18">
         <v>15</v>
       </c>
@@ -1428,7 +1674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="18"/>
       <c r="C15" s="18">
         <v>14</v>
@@ -1448,8 +1694,11 @@
       <c r="K15" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="19"/>
       <c r="C16" s="19">
         <v>15</v>
@@ -1469,8 +1718,11 @@
       <c r="K16" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B17" s="13"/>
       <c r="I17" s="1" t="s">
         <v>23</v>
@@ -1481,8 +1733,11 @@
       <c r="K17" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1492,8 +1747,11 @@
       <c r="K18" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1503,60 +1761,72 @@
       <c r="K19" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="49"/>
+      <c r="E20" s="76"/>
       <c r="F20" s="43" t="s">
         <v>81</v>
       </c>
       <c r="G20" s="30"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="73" t="s">
+      <c r="F21" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="31"/>
-      <c r="I21" s="45" t="s">
+      <c r="G21" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="I21" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="45" t="s">
+      <c r="J21" s="54" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
         <v>1</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="73" t="s">
+      <c r="F22" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="31"/>
+      <c r="G22" s="31" t="s">
+        <v>137</v>
+      </c>
       <c r="I22" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="J22" s="72" t="s">
+      <c r="J22" s="52" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="M22" s="90"/>
+      <c r="N22" s="90"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B23" s="20">
         <v>2</v>
       </c>
@@ -1565,15 +1835,24 @@
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
       <c r="G23" s="33"/>
-      <c r="H23" s="71"/>
+      <c r="H23" s="51"/>
       <c r="I23" s="45" t="s">
         <v>50</v>
       </c>
       <c r="J23" s="45" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="M23" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="N23" s="29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B24" s="20">
         <v>3</v>
       </c>
@@ -1588,21 +1867,30 @@
       <c r="J24" s="22" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="M24" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="N24" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B25" s="10">
         <v>4</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="57" t="s">
+      <c r="D25" s="70" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="73" t="s">
+      <c r="F25" s="53" t="s">
         <v>85</v>
       </c>
       <c r="G25" s="33"/>
@@ -1612,20 +1900,29 @@
       <c r="J25" s="22" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="68" t="s">
+      <c r="L25" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="M25" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="N25" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="69">
+      <c r="B26" s="49">
         <v>5</v>
       </c>
-      <c r="C26" s="55"/>
-      <c r="D26" s="57"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="70"/>
       <c r="E26" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="73" t="s">
+      <c r="F26" s="53" t="s">
         <v>86</v>
       </c>
       <c r="G26" s="33"/>
@@ -1635,17 +1932,29 @@
       <c r="J26" s="45" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="M26" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="N26" s="86" t="s">
+        <v>148</v>
+      </c>
+      <c r="O26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <v>6</v>
       </c>
-      <c r="C27" s="55"/>
-      <c r="D27" s="57"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="70"/>
       <c r="E27" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="73" t="s">
+      <c r="F27" s="53" t="s">
         <v>87</v>
       </c>
       <c r="G27" s="33"/>
@@ -1655,17 +1964,29 @@
       <c r="J27" s="45" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="M27" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="N27" s="86" t="s">
+        <v>148</v>
+      </c>
+      <c r="O27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B28" s="10">
         <v>7</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="57"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="73" t="s">
+      <c r="F28" s="53" t="s">
         <v>88</v>
       </c>
       <c r="G28" s="33"/>
@@ -1675,15 +1996,24 @@
       <c r="J28" s="45" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" s="83" t="s">
+        <v>109</v>
+      </c>
+      <c r="M28" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="N28" s="87" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B29" s="10">
         <v>8</v>
       </c>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="57"/>
+      <c r="D29" s="70"/>
       <c r="E29" s="38" t="s">
         <v>42</v>
       </c>
@@ -1695,13 +2025,22 @@
       <c r="J29" s="45" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29" s="83" t="s">
+        <v>111</v>
+      </c>
+      <c r="M29" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="N29" s="87" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B30" s="10">
         <v>9</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="57"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="70"/>
       <c r="E30" s="38" t="s">
         <v>43</v>
       </c>
@@ -1713,17 +2052,26 @@
       <c r="J30" s="45" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="M30" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="N30" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B31" s="10">
         <v>10</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="57"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="70"/>
       <c r="E31" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="70"/>
+      <c r="F31" s="50"/>
       <c r="G31" s="33"/>
       <c r="I31" s="45" t="s">
         <v>58</v>
@@ -1731,13 +2079,22 @@
       <c r="J31" s="45" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="M31" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="N31" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>11</v>
       </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="57"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="70"/>
       <c r="E32" s="38" t="s">
         <v>45</v>
       </c>
@@ -1749,8 +2106,17 @@
       <c r="J32" s="45" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L32" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="M32" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="N32" s="86" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="10">
         <v>12</v>
       </c>
@@ -1765,8 +2131,17 @@
       <c r="J33" s="45" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L33" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="M33" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="N33" s="86" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" s="20">
         <v>13</v>
       </c>
@@ -1781,8 +2156,17 @@
       <c r="J34" s="45" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L34" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="M34" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="N34" s="86" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" s="20">
         <v>14</v>
       </c>
@@ -1797,8 +2181,17 @@
       <c r="J35" s="45" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L35" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="M35" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="N35" s="86" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="10">
         <v>15</v>
       </c>
@@ -1813,56 +2206,116 @@
       <c r="J36" s="45" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L36" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="M36" s="82" t="s">
+        <v>110</v>
+      </c>
+      <c r="N36" s="88" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="I37" s="45" t="s">
         <v>64</v>
       </c>
       <c r="J37" s="45" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L37" s="81" t="s">
+        <v>126</v>
+      </c>
+      <c r="M37" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="N37" s="88" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L38" s="81" t="s">
+        <v>127</v>
+      </c>
+      <c r="M38" s="82" t="s">
+        <v>114</v>
+      </c>
+      <c r="N38" s="88" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="62" t="s">
+      <c r="D39" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="62"/>
+      <c r="E39" s="75"/>
       <c r="F39" s="45" t="s">
         <v>81</v>
       </c>
       <c r="G39" s="29"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L39" s="81" t="s">
+        <v>128</v>
+      </c>
+      <c r="M39" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="N39" s="88" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" s="11">
         <v>0</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="73" t="s">
+      <c r="F40" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="G40" s="31"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G40" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="L40" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="M40" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="N40" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="73" t="s">
+      <c r="F41" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="G41" s="31"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G41" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="L41" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="M41" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="N41" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
         <v>2</v>
       </c>
@@ -1871,8 +2324,17 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="31"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L42" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="M42" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="N42" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B43" s="22">
         <v>3</v>
       </c>
@@ -1881,87 +2343,126 @@
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
       <c r="G43" s="35"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="L43" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="M43" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="N43" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B44" s="11">
         <v>4</v>
       </c>
       <c r="C44" s="11"/>
-      <c r="D44" s="61" t="s">
+      <c r="D44" s="74" t="s">
         <v>28</v>
       </c>
       <c r="E44" s="39" t="s">
         <v>30</v>
       </c>
       <c r="F44" s="41"/>
-      <c r="G44" s="33"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G44" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="L44" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="M44" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="N44" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
         <v>5</v>
       </c>
       <c r="C45" s="11"/>
-      <c r="D45" s="61"/>
+      <c r="D45" s="74"/>
       <c r="E45" s="39" t="s">
         <v>31</v>
       </c>
       <c r="F45" s="41"/>
-      <c r="G45" s="33"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G45" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="L45" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="M45" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="N45" s="85" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B46" s="11">
         <v>6</v>
       </c>
       <c r="C46" s="11"/>
-      <c r="D46" s="61"/>
+      <c r="D46" s="74"/>
       <c r="E46" s="39" t="s">
         <v>32</v>
       </c>
       <c r="F46" s="41"/>
-      <c r="G46" s="33"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G46" s="33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <v>7</v>
       </c>
       <c r="C47" s="11"/>
-      <c r="D47" s="61"/>
+      <c r="D47" s="74"/>
       <c r="E47" s="39" t="s">
         <v>36</v>
       </c>
       <c r="F47" s="41"/>
-      <c r="G47" s="33"/>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G47" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
         <v>8</v>
       </c>
       <c r="C48" s="11"/>
-      <c r="D48" s="61"/>
+      <c r="D48" s="74"/>
       <c r="E48" s="39" t="s">
         <v>35</v>
       </c>
       <c r="F48" s="41"/>
-      <c r="G48" s="33"/>
+      <c r="G48" s="33" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" s="11">
         <v>9</v>
       </c>
       <c r="C49" s="11"/>
-      <c r="D49" s="61"/>
+      <c r="D49" s="74"/>
       <c r="E49" s="39" t="s">
         <v>34</v>
       </c>
       <c r="F49" s="41"/>
-      <c r="G49" s="33"/>
+      <c r="G49" s="33" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="11">
         <v>10</v>
       </c>
       <c r="C50" s="11"/>
-      <c r="D50" s="61"/>
+      <c r="D50" s="74"/>
       <c r="E50" s="39" t="s">
         <v>33</v>
       </c>
@@ -1982,7 +2483,7 @@
       <c r="B52" s="11">
         <v>12</v>
       </c>
-      <c r="C52" s="58" t="s">
+      <c r="C52" s="71" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="24"/>
@@ -1994,7 +2495,7 @@
       <c r="B53" s="11">
         <v>13</v>
       </c>
-      <c r="C53" s="59"/>
+      <c r="C53" s="72"/>
       <c r="D53" s="24"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2004,7 +2505,7 @@
       <c r="B54" s="11">
         <v>14</v>
       </c>
-      <c r="C54" s="59"/>
+      <c r="C54" s="72"/>
       <c r="D54" s="24"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2014,7 +2515,7 @@
       <c r="B55" s="11">
         <v>15</v>
       </c>
-      <c r="C55" s="60"/>
+      <c r="C55" s="73"/>
       <c r="D55" s="24"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2030,15 +2531,15 @@
       <c r="D58" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="63" t="s">
+      <c r="E58" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="F58" s="64"/>
-      <c r="G58" s="62" t="s">
+      <c r="F58" s="78"/>
+      <c r="G58" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="H58" s="62"/>
-      <c r="I58" s="67" t="s">
+      <c r="H58" s="75"/>
+      <c r="I58" s="47" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2046,17 +2547,17 @@
       <c r="B59" s="11">
         <v>0</v>
       </c>
-      <c r="C59" s="53" t="s">
+      <c r="C59" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="54" t="s">
+      <c r="D59" s="67" t="s">
         <v>14</v>
       </c>
       <c r="E59" s="24"/>
       <c r="F59" s="24"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="73" t="s">
+      <c r="I59" s="53" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2064,13 +2565,13 @@
       <c r="B60" s="11">
         <v>1</v>
       </c>
-      <c r="C60" s="53"/>
-      <c r="D60" s="54"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="67"/>
       <c r="E60" s="24"/>
       <c r="F60" s="24"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="73" t="s">
+      <c r="I60" s="53" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2078,13 +2579,13 @@
       <c r="B61" s="11">
         <v>2</v>
       </c>
-      <c r="C61" s="53"/>
-      <c r="D61" s="54"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="67"/>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="73" t="s">
+      <c r="I61" s="53" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2092,13 +2593,13 @@
       <c r="B62" s="11">
         <v>3</v>
       </c>
-      <c r="C62" s="53"/>
-      <c r="D62" s="54"/>
+      <c r="C62" s="66"/>
+      <c r="D62" s="67"/>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="73" t="s">
+      <c r="I62" s="53" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2106,13 +2607,13 @@
       <c r="B63" s="11">
         <v>4</v>
       </c>
-      <c r="C63" s="53"/>
+      <c r="C63" s="66"/>
       <c r="D63" s="23"/>
       <c r="E63" s="24"/>
       <c r="F63" s="24"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="73" t="s">
+      <c r="I63" s="53" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2120,9 +2621,9 @@
       <c r="B64" s="11">
         <v>5</v>
       </c>
-      <c r="C64" s="53"/>
+      <c r="C64" s="66"/>
       <c r="D64" s="24"/>
-      <c r="E64" s="65" t="s">
+      <c r="E64" s="79" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="32" t="s">
@@ -2130,7 +2631,7 @@
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="73" t="s">
+      <c r="I64" s="53" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2138,13 +2639,13 @@
       <c r="B65" s="11">
         <v>6</v>
       </c>
-      <c r="C65" s="53"/>
+      <c r="C65" s="66"/>
       <c r="D65" s="24"/>
-      <c r="E65" s="66"/>
+      <c r="E65" s="80"/>
       <c r="F65" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G65" s="46" t="s">
+      <c r="G65" s="59" t="s">
         <v>28</v>
       </c>
       <c r="H65" s="37" t="s">
@@ -2156,13 +2657,13 @@
       <c r="B66" s="11">
         <v>7</v>
       </c>
-      <c r="C66" s="53"/>
+      <c r="C66" s="66"/>
       <c r="D66" s="24"/>
-      <c r="E66" s="66"/>
+      <c r="E66" s="80"/>
       <c r="F66" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G66" s="47"/>
+      <c r="G66" s="60"/>
       <c r="H66" s="37" t="s">
         <v>31</v>
       </c>
@@ -2174,11 +2675,11 @@
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="66"/>
+      <c r="E67" s="80"/>
       <c r="F67" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="G67" s="47"/>
+      <c r="G67" s="60"/>
       <c r="H67" s="37" t="s">
         <v>32</v>
       </c>
@@ -2190,11 +2691,11 @@
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
-      <c r="E68" s="66"/>
+      <c r="E68" s="80"/>
       <c r="F68" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="G68" s="47"/>
+      <c r="G68" s="60"/>
       <c r="H68" s="37" t="s">
         <v>36</v>
       </c>
@@ -2206,11 +2707,11 @@
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
-      <c r="E69" s="66"/>
+      <c r="E69" s="80"/>
       <c r="F69" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="G69" s="47"/>
+      <c r="G69" s="60"/>
       <c r="H69" s="37" t="s">
         <v>35</v>
       </c>
@@ -2222,11 +2723,11 @@
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
-      <c r="E70" s="66"/>
+      <c r="E70" s="80"/>
       <c r="F70" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="G70" s="47"/>
+      <c r="G70" s="60"/>
       <c r="H70" s="37" t="s">
         <v>34</v>
       </c>
@@ -2238,11 +2739,11 @@
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
-      <c r="E71" s="66"/>
+      <c r="E71" s="80"/>
       <c r="F71" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G71" s="48"/>
+      <c r="G71" s="61"/>
       <c r="H71" s="37" t="s">
         <v>33</v>
       </c>
@@ -2298,7 +2799,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="L22:N22"/>
     <mergeCell ref="G65:G71"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
ready to test functions for PWM tim4 and TIM5, TIM3 done
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -442,9 +442,6 @@
     <t>Pin_B9</t>
   </si>
   <si>
-    <t>probar si funciona encender algo con estos pines</t>
-  </si>
-  <si>
     <t>PWM_TIM5_CH1</t>
   </si>
   <si>
@@ -482,6 +479,9 @@
   </si>
   <si>
     <t>AF2,AF3</t>
+  </si>
+  <si>
+    <t>Function 4</t>
   </si>
 </sst>
 </file>
@@ -636,7 +636,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -939,19 +939,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1002,6 +990,24 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1068,35 +1074,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1419,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O78"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E28" zoomScale="153" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="I14" zoomScale="153" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1722,7 +1709,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B17" s="13"/>
       <c r="I17" s="1" t="s">
         <v>23</v>
@@ -1737,7 +1724,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1751,7 +1738,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1765,7 +1752,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1776,57 +1763,59 @@
         <v>9</v>
       </c>
       <c r="E20" s="76"/>
-      <c r="F20" s="43" t="s">
+      <c r="F20" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="30"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G20" s="54" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B21" s="10">
         <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="53" t="s">
+      <c r="F21" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="I21" s="54" t="s">
+      <c r="G21" s="82" t="s">
+        <v>135</v>
+      </c>
+      <c r="I21" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="54" t="s">
+      <c r="J21" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B22" s="10">
         <v>1</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="53" t="s">
+      <c r="F22" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="I22" s="45" t="s">
+      <c r="G22" s="82" t="s">
+        <v>136</v>
+      </c>
+      <c r="I22" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="J22" s="52" t="s">
+      <c r="J22" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="L22" s="89" t="s">
+      <c r="L22" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="M22" s="90"/>
-      <c r="N22" s="90"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M22" s="58"/>
+      <c r="N22" s="58"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B23" s="20">
         <v>2</v>
       </c>
@@ -1834,25 +1823,25 @@
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="45" t="s">
+      <c r="G23" s="21"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="J23" s="45" t="s">
+      <c r="J23" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="L23" s="46" t="s">
+      <c r="L23" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="M23" s="46" t="s">
+      <c r="M23" s="40" t="s">
         <v>100</v>
       </c>
       <c r="N23" s="29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" s="20">
         <v>3</v>
       </c>
@@ -1860,24 +1849,24 @@
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
-      <c r="G24" s="34"/>
+      <c r="G24" s="81"/>
       <c r="I24" s="22" t="s">
         <v>51</v>
       </c>
       <c r="J24" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="L24" s="58" t="s">
+      <c r="L24" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="M24" s="57" t="s">
+      <c r="M24" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="N24" s="85" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N24" s="55" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" s="10">
         <v>4</v>
       </c>
@@ -1887,113 +1876,107 @@
       <c r="D25" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="53" t="s">
+      <c r="F25" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="33"/>
+      <c r="G25" s="35"/>
       <c r="I25" s="22" t="s">
         <v>52</v>
       </c>
       <c r="J25" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="L25" s="58" t="s">
+      <c r="L25" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="M25" s="57" t="s">
+      <c r="M25" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="N25" s="85" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="48" t="s">
+      <c r="N25" s="55" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="49">
+      <c r="B26" s="43">
         <v>5</v>
       </c>
       <c r="C26" s="68"/>
       <c r="D26" s="70"/>
-      <c r="E26" s="38" t="s">
+      <c r="E26" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="53" t="s">
+      <c r="F26" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="I26" s="45" t="s">
+      <c r="G26" s="35"/>
+      <c r="I26" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="J26" s="45" t="s">
+      <c r="J26" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="L26" s="55" t="s">
+      <c r="L26" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="M26" s="56" t="s">
+      <c r="M26" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="N26" s="86" t="s">
-        <v>148</v>
-      </c>
-      <c r="O26" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N26" s="56" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="10">
         <v>6</v>
       </c>
       <c r="C27" s="68"/>
       <c r="D27" s="70"/>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="53" t="s">
+      <c r="F27" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="33"/>
-      <c r="I27" s="45" t="s">
+      <c r="G27" s="35"/>
+      <c r="I27" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="J27" s="45" t="s">
+      <c r="J27" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="L27" s="55" t="s">
+      <c r="L27" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="M27" s="56" t="s">
+      <c r="M27" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="N27" s="86" t="s">
-        <v>148</v>
-      </c>
-      <c r="O27" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N27" s="56" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B28" s="10">
         <v>7</v>
       </c>
       <c r="C28" s="68"/>
       <c r="D28" s="70"/>
-      <c r="E28" s="38" t="s">
+      <c r="E28" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="53" t="s">
+      <c r="F28" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="33"/>
-      <c r="I28" s="45" t="s">
+      <c r="G28" s="35"/>
+      <c r="I28" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="J28" s="45" t="s">
+      <c r="J28" s="39" t="s">
         <v>77</v>
       </c>
       <c r="L28" s="83" t="s">
@@ -2002,11 +1985,11 @@
       <c r="M28" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="N28" s="87" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N28" s="85" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" s="10">
         <v>8</v>
       </c>
@@ -2014,15 +1997,15 @@
         <v>10</v>
       </c>
       <c r="D29" s="70"/>
-      <c r="E29" s="38" t="s">
+      <c r="E29" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="F29" s="41"/>
-      <c r="G29" s="33"/>
-      <c r="I29" s="45" t="s">
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="I29" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="J29" s="45" t="s">
+      <c r="J29" s="39" t="s">
         <v>78</v>
       </c>
       <c r="L29" s="83" t="s">
@@ -2031,89 +2014,89 @@
       <c r="M29" s="84" t="s">
         <v>112</v>
       </c>
-      <c r="N29" s="87" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N29" s="85" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B30" s="10">
         <v>9</v>
       </c>
       <c r="C30" s="69"/>
       <c r="D30" s="70"/>
-      <c r="E30" s="38" t="s">
+      <c r="E30" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F30" s="41"/>
-      <c r="G30" s="33"/>
-      <c r="I30" s="45" t="s">
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="I30" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="J30" s="45" t="s">
+      <c r="J30" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="L30" s="58" t="s">
+      <c r="L30" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="M30" s="57" t="s">
+      <c r="M30" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="N30" s="85" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N30" s="55" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B31" s="10">
         <v>10</v>
       </c>
       <c r="C31" s="69"/>
       <c r="D31" s="70"/>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="50"/>
-      <c r="G31" s="33"/>
-      <c r="I31" s="45" t="s">
+      <c r="F31" s="44"/>
+      <c r="G31" s="35"/>
+      <c r="I31" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="J31" s="45" t="s">
+      <c r="J31" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="L31" s="58" t="s">
+      <c r="L31" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="M31" s="57" t="s">
+      <c r="M31" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="N31" s="85" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N31" s="55" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B32" s="10">
         <v>11</v>
       </c>
       <c r="C32" s="69"/>
       <c r="D32" s="70"/>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="33"/>
-      <c r="I32" s="45" t="s">
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="I32" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="J32" s="45" t="s">
+      <c r="J32" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="L32" s="55" t="s">
+      <c r="L32" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="M32" s="56" t="s">
+      <c r="M32" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="N32" s="86" t="s">
-        <v>147</v>
+      <c r="N32" s="56" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
@@ -2123,22 +2106,22 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="33"/>
-      <c r="I33" s="45" t="s">
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="I33" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="J33" s="45" t="s">
+      <c r="J33" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="L33" s="55" t="s">
+      <c r="L33" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="M33" s="56" t="s">
+      <c r="M33" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="N33" s="86" t="s">
-        <v>147</v>
+      <c r="N33" s="56" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
@@ -2149,21 +2132,21 @@
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
       <c r="F34" s="21"/>
-      <c r="G34" s="33"/>
-      <c r="I34" s="45" t="s">
+      <c r="G34" s="21"/>
+      <c r="I34" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="J34" s="45" t="s">
+      <c r="J34" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="L34" s="55" t="s">
+      <c r="L34" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="M34" s="56" t="s">
+      <c r="M34" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="N34" s="86" t="s">
-        <v>147</v>
+      <c r="N34" s="56" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
@@ -2174,21 +2157,21 @@
       <c r="D35" s="21"/>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
-      <c r="G35" s="33"/>
-      <c r="I35" s="45" t="s">
+      <c r="G35" s="21"/>
+      <c r="I35" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="J35" s="45" t="s">
+      <c r="J35" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="L35" s="55" t="s">
+      <c r="L35" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="M35" s="56" t="s">
+      <c r="M35" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="N35" s="86" t="s">
-        <v>147</v>
+      <c r="N35" s="56" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
@@ -2198,50 +2181,50 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="33"/>
-      <c r="I36" s="45" t="s">
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="I36" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="J36" s="45" t="s">
+      <c r="J36" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="L36" s="81" t="s">
+      <c r="L36" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="M36" s="82" t="s">
+      <c r="M36" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="N36" s="88" t="s">
-        <v>147</v>
+      <c r="N36" s="56" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="I37" s="45" t="s">
+      <c r="I37" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="J37" s="45" t="s">
+      <c r="J37" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="L37" s="81" t="s">
+      <c r="L37" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="M37" s="82" t="s">
+      <c r="M37" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="N37" s="88" t="s">
-        <v>147</v>
+      <c r="N37" s="56" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="L38" s="81" t="s">
+      <c r="L38" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="M38" s="82" t="s">
+      <c r="M38" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="N38" s="88" t="s">
-        <v>147</v>
+      <c r="N38" s="56" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.3">
@@ -2255,18 +2238,20 @@
         <v>9</v>
       </c>
       <c r="E39" s="75"/>
-      <c r="F39" s="45" t="s">
+      <c r="F39" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="G39" s="29"/>
-      <c r="L39" s="81" t="s">
+      <c r="G39" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="L39" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="M39" s="82" t="s">
+      <c r="M39" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="N39" s="88" t="s">
-        <v>147</v>
+      <c r="N39" s="56" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.3">
@@ -2276,20 +2261,20 @@
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="53" t="s">
+      <c r="F40" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="G40" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="L40" s="58" t="s">
+      <c r="G40" s="82" t="s">
+        <v>137</v>
+      </c>
+      <c r="L40" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="M40" s="57" t="s">
+      <c r="M40" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="N40" s="85" t="s">
-        <v>147</v>
+      <c r="N40" s="55" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.3">
@@ -2299,20 +2284,20 @@
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="53" t="s">
+      <c r="F41" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="G41" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="L41" s="58" t="s">
+      <c r="G41" s="82" t="s">
+        <v>138</v>
+      </c>
+      <c r="L41" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="M41" s="57" t="s">
+      <c r="M41" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="N41" s="85" t="s">
-        <v>147</v>
+      <c r="N41" s="55" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.3">
@@ -2323,15 +2308,15 @@
       <c r="D42" s="11"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="31"/>
-      <c r="L42" s="58" t="s">
+      <c r="G42" s="1"/>
+      <c r="L42" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="M42" s="57" t="s">
+      <c r="M42" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="N42" s="85" t="s">
-        <v>147</v>
+      <c r="N42" s="55" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.3">
@@ -2342,15 +2327,15 @@
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
-      <c r="G43" s="35"/>
-      <c r="L43" s="58" t="s">
+      <c r="G43" s="22"/>
+      <c r="L43" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="M43" s="57" t="s">
+      <c r="M43" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="N43" s="85" t="s">
-        <v>147</v>
+      <c r="N43" s="55" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.3">
@@ -2361,21 +2346,21 @@
       <c r="D44" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="39" t="s">
+      <c r="E44" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F44" s="41"/>
-      <c r="G44" s="33" t="s">
-        <v>140</v>
-      </c>
-      <c r="L44" s="58" t="s">
+      <c r="F44" s="35"/>
+      <c r="G44" s="82" t="s">
+        <v>139</v>
+      </c>
+      <c r="L44" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="M44" s="57" t="s">
+      <c r="M44" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="N44" s="85" t="s">
-        <v>147</v>
+      <c r="N44" s="55" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.3">
@@ -2384,21 +2369,21 @@
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="74"/>
-      <c r="E45" s="39" t="s">
+      <c r="E45" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="F45" s="41"/>
-      <c r="G45" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="L45" s="58" t="s">
+      <c r="F45" s="35"/>
+      <c r="G45" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="L45" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="M45" s="57" t="s">
+      <c r="M45" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="N45" s="85" t="s">
-        <v>147</v>
+      <c r="N45" s="55" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.3">
@@ -2407,12 +2392,12 @@
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="74"/>
-      <c r="E46" s="39" t="s">
+      <c r="E46" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F46" s="41"/>
-      <c r="G46" s="33" t="s">
-        <v>142</v>
+      <c r="F46" s="35"/>
+      <c r="G46" s="82" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.3">
@@ -2421,12 +2406,12 @@
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="74"/>
-      <c r="E47" s="39" t="s">
+      <c r="E47" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="F47" s="41"/>
-      <c r="G47" s="33" t="s">
-        <v>143</v>
+      <c r="F47" s="35"/>
+      <c r="G47" s="82" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.3">
@@ -2435,12 +2420,12 @@
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="74"/>
-      <c r="E48" s="39" t="s">
+      <c r="E48" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F48" s="41"/>
-      <c r="G48" s="33" t="s">
-        <v>144</v>
+      <c r="F48" s="35"/>
+      <c r="G48" s="82" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
@@ -2449,12 +2434,12 @@
       </c>
       <c r="C49" s="11"/>
       <c r="D49" s="74"/>
-      <c r="E49" s="39" t="s">
+      <c r="E49" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F49" s="41"/>
-      <c r="G49" s="33" t="s">
-        <v>145</v>
+      <c r="F49" s="35"/>
+      <c r="G49" s="82" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
@@ -2463,11 +2448,11 @@
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="74"/>
-      <c r="E50" s="39" t="s">
+      <c r="E50" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="F50" s="41"/>
-      <c r="G50" s="33"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="25">
@@ -2477,7 +2462,7 @@
       <c r="D51" s="27"/>
       <c r="E51" s="27"/>
       <c r="F51" s="27"/>
-      <c r="G51" s="36"/>
+      <c r="G51" s="27"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
@@ -2489,7 +2474,7 @@
       <c r="D52" s="24"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="31"/>
+      <c r="G52" s="1"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="11">
@@ -2499,7 +2484,7 @@
       <c r="D53" s="24"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="31"/>
+      <c r="G53" s="1"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
@@ -2509,7 +2494,7 @@
       <c r="D54" s="24"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="31"/>
+      <c r="G54" s="1"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
@@ -2519,7 +2504,7 @@
       <c r="D55" s="24"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="31"/>
+      <c r="G55" s="1"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" s="11" t="s">
@@ -2539,7 +2524,7 @@
         <v>29</v>
       </c>
       <c r="H58" s="75"/>
-      <c r="I58" s="47" t="s">
+      <c r="I58" s="41" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2557,7 +2542,7 @@
       <c r="F59" s="24"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="53" t="s">
+      <c r="I59" s="47" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2571,7 +2556,7 @@
       <c r="F60" s="24"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="53" t="s">
+      <c r="I60" s="47" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2585,7 +2570,7 @@
       <c r="F61" s="24"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="53" t="s">
+      <c r="I61" s="47" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2599,7 +2584,7 @@
       <c r="F62" s="24"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="53" t="s">
+      <c r="I62" s="47" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2613,7 +2598,7 @@
       <c r="F63" s="24"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="53" t="s">
+      <c r="I63" s="47" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2626,12 +2611,12 @@
       <c r="E64" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="F64" s="32" t="s">
+      <c r="F64" s="30" t="s">
         <v>38</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="53" t="s">
+      <c r="I64" s="47" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2642,13 +2627,13 @@
       <c r="C65" s="66"/>
       <c r="D65" s="24"/>
       <c r="E65" s="80"/>
-      <c r="F65" s="32" t="s">
+      <c r="F65" s="30" t="s">
         <v>39</v>
       </c>
       <c r="G65" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="H65" s="37" t="s">
+      <c r="H65" s="31" t="s">
         <v>30</v>
       </c>
       <c r="I65" s="1"/>
@@ -2660,11 +2645,11 @@
       <c r="C66" s="66"/>
       <c r="D66" s="24"/>
       <c r="E66" s="80"/>
-      <c r="F66" s="32" t="s">
+      <c r="F66" s="30" t="s">
         <v>40</v>
       </c>
       <c r="G66" s="60"/>
-      <c r="H66" s="37" t="s">
+      <c r="H66" s="31" t="s">
         <v>31</v>
       </c>
       <c r="I66" s="1"/>
@@ -2676,11 +2661,11 @@
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="80"/>
-      <c r="F67" s="32" t="s">
+      <c r="F67" s="30" t="s">
         <v>41</v>
       </c>
       <c r="G67" s="60"/>
-      <c r="H67" s="37" t="s">
+      <c r="H67" s="31" t="s">
         <v>32</v>
       </c>
       <c r="I67" s="1"/>
@@ -2692,11 +2677,11 @@
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
       <c r="E68" s="80"/>
-      <c r="F68" s="32" t="s">
+      <c r="F68" s="30" t="s">
         <v>42</v>
       </c>
       <c r="G68" s="60"/>
-      <c r="H68" s="37" t="s">
+      <c r="H68" s="31" t="s">
         <v>36</v>
       </c>
       <c r="I68" s="1"/>
@@ -2708,11 +2693,11 @@
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
       <c r="E69" s="80"/>
-      <c r="F69" s="32" t="s">
+      <c r="F69" s="30" t="s">
         <v>43</v>
       </c>
       <c r="G69" s="60"/>
-      <c r="H69" s="37" t="s">
+      <c r="H69" s="31" t="s">
         <v>35</v>
       </c>
       <c r="I69" s="1"/>
@@ -2724,11 +2709,11 @@
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
       <c r="E70" s="80"/>
-      <c r="F70" s="32" t="s">
+      <c r="F70" s="30" t="s">
         <v>44</v>
       </c>
       <c r="G70" s="60"/>
-      <c r="H70" s="37" t="s">
+      <c r="H70" s="31" t="s">
         <v>34</v>
       </c>
       <c r="I70" s="1"/>
@@ -2740,11 +2725,11 @@
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="80"/>
-      <c r="F71" s="32" t="s">
+      <c r="F71" s="30" t="s">
         <v>45</v>
       </c>
       <c r="G71" s="61"/>
-      <c r="H71" s="37" t="s">
+      <c r="H71" s="31" t="s">
         <v>33</v>
       </c>
       <c r="I71" s="1"/>
@@ -2753,15 +2738,15 @@
       <c r="A72" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="44">
+      <c r="B72" s="38">
         <v>13</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
-      <c r="E72" s="40"/>
-      <c r="F72" s="41"/>
-      <c r="G72" s="42"/>
-      <c r="H72" s="41"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="35"/>
       <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
uart alternatives OK, WWDG and IWDG ok, update documentation, feature headers to misraC
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="154">
   <si>
     <t>Port C</t>
   </si>
@@ -430,12 +430,6 @@
     <t>Pin_B9</t>
   </si>
   <si>
-    <t>PWM_TIM5_CH1</t>
-  </si>
-  <si>
-    <t>PWM_TIM5_CH2</t>
-  </si>
-  <si>
     <t>PWM_TIM3_CH3</t>
   </si>
   <si>
@@ -476,6 +470,33 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>PWM_TIM5_CH1(P)</t>
+  </si>
+  <si>
+    <t>PWM_TIM5_CH2 (P)</t>
+  </si>
+  <si>
+    <t>UART1 TX</t>
+  </si>
+  <si>
+    <t>UART6 TX</t>
+  </si>
+  <si>
+    <t>UART1 RX</t>
+  </si>
+  <si>
+    <t>Function 6</t>
+  </si>
+  <si>
+    <t>UART6 RX</t>
+  </si>
+  <si>
+    <t>UART2 TX (only 4 uart)</t>
+  </si>
+  <si>
+    <t>UART2 RX (only 4 uart)</t>
   </si>
 </sst>
 </file>
@@ -507,7 +528,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -625,6 +646,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,7 +878,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -939,7 +966,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -977,15 +1003,67 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1001,58 +1079,27 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1081,7 +1128,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>780728</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>51982</xdr:rowOff>
@@ -1383,7 +1430,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>666901</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>140488</xdr:rowOff>
@@ -1648,7 +1695,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>284964</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>90912</xdr:rowOff>
@@ -1844,7 +1891,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>554790</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>160422</xdr:rowOff>
@@ -2067,13 +2114,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>456562</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>47510</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>749504</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>82280</xdr:rowOff>
@@ -2105,7 +2152,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>12225</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>62712</xdr:rowOff>
@@ -2462,7 +2509,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>390071</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>165257</xdr:rowOff>
@@ -2671,7 +2718,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>682882</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>90872</xdr:rowOff>
@@ -3042,7 +3089,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>756478</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>101364</xdr:rowOff>
@@ -3406,7 +3453,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>73124</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>4496</xdr:rowOff>
@@ -3763,7 +3810,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>755453</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>44726</xdr:rowOff>
@@ -3832,7 +3879,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>719010</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>37075</xdr:rowOff>
@@ -3901,14 +3948,14 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>194553</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>129702</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>583174</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>583175</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>4702</xdr:rowOff>
     </xdr:to>
@@ -3934,8 +3981,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="14559064" y="7133617"/>
-          <a:ext cx="5949599" cy="4690191"/>
+          <a:off x="16315616" y="7307470"/>
+          <a:ext cx="5936934" cy="4834803"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4254,18 +4301,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O78"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="111" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="R52" zoomScale="224" workbookViewId="0">
+      <selection activeCell="F65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
     <col min="9" max="9" width="15.109375" customWidth="1"/>
     <col min="10" max="10" width="16.44140625" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" customWidth="1"/>
@@ -4273,19 +4320,20 @@
     <col min="13" max="14" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="61" t="s">
+    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="63"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="21"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
@@ -4301,7 +4349,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="11">
         <v>0</v>
       </c>
@@ -4316,13 +4364,15 @@
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="22"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="11">
         <v>1</v>
       </c>
@@ -4335,13 +4385,15 @@
       <c r="E4" s="11"/>
       <c r="F4" s="22"/>
       <c r="G4" s="22"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="11">
         <v>4</v>
       </c>
@@ -4354,13 +4406,15 @@
       <c r="E5" s="11"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="11">
         <v>5</v>
       </c>
@@ -4373,13 +4427,15 @@
       <c r="E6" s="11"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="11">
         <v>6</v>
       </c>
@@ -4392,8 +4448,10 @@
       <c r="E7" s="11"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>7</v>
       </c>
@@ -4406,8 +4464,10 @@
       <c r="E8" s="11"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="11">
         <v>8</v>
       </c>
@@ -4420,8 +4480,10 @@
       <c r="E9" s="11"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="11">
         <v>9</v>
       </c>
@@ -4434,8 +4496,10 @@
       <c r="E10" s="11"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="11">
         <v>10</v>
       </c>
@@ -4448,8 +4512,10 @@
       <c r="E11" s="11"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
         <v>11</v>
       </c>
@@ -4462,8 +4528,10 @@
       <c r="E12" s="11"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="11">
         <v>12</v>
       </c>
@@ -4476,15 +4544,17 @@
       <c r="E13" s="11"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="I13" s="56" t="s">
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="K13" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="56"/>
-      <c r="M13" s="56"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <v>15</v>
       </c>
@@ -4497,21 +4567,23 @@
       <c r="E14" s="11"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
-      <c r="I14" s="1" t="s">
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="K14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="55" t="s">
-        <v>145</v>
-      </c>
-      <c r="M14" s="55"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N14" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="O14" s="68"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="11"/>
       <c r="C15" s="11">
         <v>14</v>
@@ -4522,21 +4594,23 @@
       <c r="E15" s="11"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
-      <c r="I15" s="1" t="s">
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="K15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="1">
+      <c r="L15" s="1">
         <v>16</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="12"/>
       <c r="C16" s="12">
         <v>15</v>
@@ -4547,136 +4621,143 @@
       <c r="E16" s="12"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="I16" s="1" t="s">
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="K16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="1">
+      <c r="L16" s="1">
         <v>32</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
-      <c r="I17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="1">
+      <c r="L17" s="1">
         <v>16</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I18" s="1" t="s">
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="1">
+      <c r="L18" s="1">
         <v>16</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I19" s="1" t="s">
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="1">
+      <c r="L19" s="1">
         <v>16</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="55"/>
+      <c r="E20" s="68"/>
       <c r="F20" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="G20" s="46" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G20" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="H20" s="84" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="79"/>
+      <c r="J20" s="51"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="G21" s="78" t="s">
-        <v>131</v>
-      </c>
-      <c r="H21" t="s">
-        <v>146</v>
-      </c>
-      <c r="I21" s="40" t="s">
+      <c r="G21" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="40" t="s">
+      <c r="L21" s="39" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>1</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="G22" s="78" t="s">
-        <v>132</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="G22" s="54" t="s">
         <v>146</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="H22" s="28"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="38" t="s">
+      <c r="L22" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="L22" s="57" t="s">
+      <c r="N22" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O22" s="74"/>
+      <c r="P22" s="74"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
         <v>2</v>
       </c>
@@ -4685,24 +4766,28 @@
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="32" t="s">
+      <c r="H23" s="85" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23" s="78"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="J23" s="32" t="s">
+      <c r="L23" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="L23" s="51" t="s">
+      <c r="N23" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="M23" s="51" t="s">
+      <c r="O23" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="N23" s="51" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23" s="50" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B24" s="13">
         <v>3</v>
       </c>
@@ -4710,263 +4795,292 @@
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="47"/>
-      <c r="I24" s="15" t="s">
+      <c r="G24" s="46"/>
+      <c r="H24" s="86" t="s">
+        <v>153</v>
+      </c>
+      <c r="I24" s="81"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="J24" s="15" t="s">
+      <c r="L24" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="L24" s="76" t="s">
+      <c r="N24" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="M24" s="77" t="s">
+      <c r="O24" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="N24" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="O24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <v>4</v>
       </c>
-      <c r="C25" s="66" t="s">
+      <c r="C25" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="68" t="s">
+      <c r="D25" s="62" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="38" t="s">
         <v>81</v>
       </c>
       <c r="G25" s="28"/>
-      <c r="I25" s="15" t="s">
+      <c r="H25" s="28"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="L25" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="L25" s="76" t="s">
+      <c r="N25" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="M25" s="77" t="s">
+      <c r="O25" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="N25" s="77" t="s">
-        <v>142</v>
-      </c>
-      <c r="O25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P25" s="53" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="34" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="35">
         <v>5</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="68"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="62"/>
       <c r="E26" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="39" t="s">
+      <c r="F26" s="38" t="s">
         <v>82</v>
       </c>
       <c r="G26" s="28"/>
-      <c r="I26" s="32" t="s">
+      <c r="H26" s="28"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="J26" s="32" t="s">
+      <c r="L26" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="L26" s="41" t="s">
+      <c r="N26" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="M26" s="42" t="s">
+      <c r="O26" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="N26" s="42" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P26" s="41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <v>6</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="68"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="62"/>
       <c r="E27" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="38" t="s">
         <v>83</v>
       </c>
       <c r="G27" s="28"/>
-      <c r="I27" s="32" t="s">
+      <c r="H27" s="28"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="J27" s="32" t="s">
+      <c r="L27" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="L27" s="41" t="s">
+      <c r="N27" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="M27" s="42" t="s">
+      <c r="O27" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="N27" s="42" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27" s="41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <v>7</v>
       </c>
-      <c r="C28" s="66"/>
-      <c r="D28" s="68"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="62"/>
       <c r="E28" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="38" t="s">
         <v>84</v>
       </c>
       <c r="G28" s="28"/>
-      <c r="I28" s="32" t="s">
+      <c r="H28" s="28"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="J28" s="32" t="s">
+      <c r="L28" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="L28" s="49" t="s">
+      <c r="N28" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="M28" s="50" t="s">
+      <c r="O28" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="N28" s="50" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28" s="49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <v>8</v>
       </c>
-      <c r="C29" s="67" t="s">
+      <c r="C29" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="68"/>
+      <c r="D29" s="62"/>
       <c r="E29" s="25" t="s">
         <v>38</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
-      <c r="I29" s="32" t="s">
+      <c r="H29" s="28"/>
+      <c r="I29" s="78"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="J29" s="32" t="s">
+      <c r="L29" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="L29" s="49" t="s">
+      <c r="N29" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="M29" s="50" t="s">
+      <c r="O29" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="N29" s="50" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29" s="49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <v>9</v>
       </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="68"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="62"/>
       <c r="E30" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
-      <c r="I30" s="32" t="s">
+      <c r="H30" s="28"/>
+      <c r="I30" s="78"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="J30" s="32" t="s">
+      <c r="L30" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="L30" s="44" t="s">
+      <c r="N30" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="M30" s="43" t="s">
+      <c r="O30" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="N30" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B31" s="3">
         <v>10</v>
       </c>
-      <c r="C31" s="67"/>
-      <c r="D31" s="68"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="62"/>
       <c r="E31" s="25" t="s">
         <v>40</v>
       </c>
       <c r="F31" s="36"/>
       <c r="G31" s="28"/>
-      <c r="I31" s="32" t="s">
+      <c r="H31" s="28"/>
+      <c r="I31" s="78"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="J31" s="32" t="s">
+      <c r="L31" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="L31" s="44" t="s">
+      <c r="N31" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="M31" s="43" t="s">
+      <c r="O31" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="N31" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B32" s="3">
         <v>11</v>
       </c>
-      <c r="C32" s="67"/>
-      <c r="D32" s="68"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
       <c r="E32" s="25" t="s">
         <v>41</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
-      <c r="I32" s="32" t="s">
+      <c r="H32" s="28"/>
+      <c r="I32" s="78"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="J32" s="32" t="s">
+      <c r="L32" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="L32" s="41" t="s">
+      <c r="N32" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="M32" s="42" t="s">
+      <c r="O32" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="N32" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P32" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="3">
         <v>12</v>
       </c>
@@ -4975,23 +5089,26 @@
       <c r="E33" s="1"/>
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
-      <c r="I33" s="32" t="s">
+      <c r="H33" s="28"/>
+      <c r="I33" s="78"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="J33" s="32" t="s">
+      <c r="L33" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="L33" s="41" t="s">
+      <c r="N33" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="M33" s="42" t="s">
+      <c r="O33" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="N33" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P33" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="13">
         <v>13</v>
       </c>
@@ -5000,23 +5117,26 @@
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
-      <c r="I34" s="32" t="s">
+      <c r="H34" s="28"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="J34" s="32" t="s">
+      <c r="L34" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="L34" s="41" t="s">
+      <c r="N34" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="M34" s="42" t="s">
+      <c r="O34" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="N34" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P34" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="13">
         <v>14</v>
       </c>
@@ -5025,23 +5145,26 @@
       <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
-      <c r="I35" s="32" t="s">
+      <c r="H35" s="28"/>
+      <c r="I35" s="78"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="J35" s="32" t="s">
+      <c r="L35" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="L35" s="41" t="s">
+      <c r="N35" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="M35" s="42" t="s">
+      <c r="O35" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="N35" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P35" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="3">
         <v>15</v>
       </c>
@@ -5050,124 +5173,144 @@
       <c r="E36" s="1"/>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
-      <c r="I36" s="32" t="s">
+      <c r="H36" s="28"/>
+      <c r="I36" s="78"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="J36" s="32" t="s">
+      <c r="L36" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="L36" s="41" t="s">
+      <c r="N36" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="M36" s="42" t="s">
+      <c r="O36" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="N36" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="I37" s="32" t="s">
+      <c r="P36" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="J37" s="32" t="s">
+      <c r="L37" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="L37" s="41" t="s">
+      <c r="N37" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="M37" s="42" t="s">
+      <c r="O37" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="N37" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="L38" s="41" t="s">
+      <c r="P37" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
+      <c r="N38" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="M38" s="42" t="s">
+      <c r="O38" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="N38" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P38" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="73" t="s">
+      <c r="D39" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="73"/>
+      <c r="E39" s="67"/>
       <c r="F39" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="G39" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="L39" s="41" t="s">
+      <c r="G39" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="H39" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" s="82"/>
+      <c r="J39" s="51"/>
+      <c r="N39" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="M39" s="42" t="s">
+      <c r="O39" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="N39" s="42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P39" s="41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" s="4">
         <v>0</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="39" t="s">
+      <c r="F40" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="G40" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="L40" s="44" t="s">
+      <c r="G40" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="H40" s="28"/>
+      <c r="I40" s="78"/>
+      <c r="J40" s="51"/>
+      <c r="N40" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="M40" s="43" t="s">
+      <c r="O40" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="N40" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P40" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" s="4">
         <v>1</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="39" t="s">
+      <c r="F41" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="G41" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="L41" s="44" t="s">
+      <c r="G41" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="H41" s="28"/>
+      <c r="I41" s="78"/>
+      <c r="J41" s="51"/>
+      <c r="N41" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="M41" s="43" t="s">
+      <c r="O41" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="N41" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P41" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B42" s="4">
         <v>2</v>
       </c>
@@ -5176,17 +5319,20 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="L42" s="44" t="s">
+      <c r="H42" s="28"/>
+      <c r="I42" s="78"/>
+      <c r="J42" s="51"/>
+      <c r="N42" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="M42" s="43" t="s">
+      <c r="O42" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="N42" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P42" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B43" s="15">
         <v>3</v>
       </c>
@@ -5195,133 +5341,161 @@
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
-      <c r="L43" s="44" t="s">
+      <c r="H43" s="33"/>
+      <c r="I43" s="82"/>
+      <c r="J43" s="51"/>
+      <c r="N43" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="M43" s="43" t="s">
+      <c r="O43" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="N43" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P43" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B44" s="4">
         <v>4</v>
       </c>
       <c r="C44" s="4"/>
-      <c r="D44" s="72" t="s">
+      <c r="D44" s="66" t="s">
         <v>24</v>
       </c>
       <c r="E44" s="26" t="s">
         <v>26</v>
       </c>
       <c r="F44" s="28"/>
-      <c r="G44" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="L44" s="44" t="s">
+      <c r="G44" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="H44" s="28"/>
+      <c r="I44" s="78"/>
+      <c r="J44" s="51"/>
+      <c r="N44" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="M44" s="43" t="s">
+      <c r="O44" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="N44" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P44" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B45" s="4">
         <v>5</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="72"/>
+      <c r="D45" s="66"/>
       <c r="E45" s="26" t="s">
         <v>27</v>
       </c>
       <c r="F45" s="28"/>
-      <c r="G45" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="L45" s="44" t="s">
+      <c r="G45" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="H45" s="28"/>
+      <c r="I45" s="78"/>
+      <c r="J45" s="51"/>
+      <c r="N45" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="M45" s="43" t="s">
+      <c r="O45" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="N45" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P45" s="42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B46" s="4">
         <v>6</v>
       </c>
       <c r="C46" s="4"/>
-      <c r="D46" s="72"/>
+      <c r="D46" s="66"/>
       <c r="E46" s="26" t="s">
         <v>28</v>
       </c>
       <c r="F46" s="28"/>
-      <c r="G46" s="48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G46" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="H46" s="85" t="s">
+        <v>147</v>
+      </c>
+      <c r="I46" s="78"/>
+      <c r="J46" s="51"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B47" s="4">
         <v>7</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="72"/>
+      <c r="D47" s="66"/>
       <c r="E47" s="26" t="s">
         <v>32</v>
       </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="G47" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="H47" s="85" t="s">
+        <v>149</v>
+      </c>
+      <c r="I47" s="78"/>
+      <c r="J47" s="51"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B48" s="4">
         <v>8</v>
       </c>
       <c r="C48" s="4"/>
-      <c r="D48" s="72"/>
+      <c r="D48" s="66"/>
       <c r="E48" s="26" t="s">
         <v>31</v>
       </c>
       <c r="F48" s="28"/>
-      <c r="G48" s="48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G48" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="H48" s="28"/>
+      <c r="I48" s="78"/>
+      <c r="J48" s="51"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" s="4">
         <v>9</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="72"/>
+      <c r="D49" s="66"/>
       <c r="E49" s="26" t="s">
         <v>30</v>
       </c>
       <c r="F49" s="28"/>
-      <c r="G49" s="48" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G49" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="H49" s="28"/>
+      <c r="I49" s="78"/>
+      <c r="J49" s="51"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B50" s="4">
         <v>10</v>
       </c>
       <c r="C50" s="4"/>
-      <c r="D50" s="72"/>
+      <c r="D50" s="66"/>
       <c r="E50" s="26" t="s">
         <v>29</v>
       </c>
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H50" s="28"/>
+      <c r="I50" s="78"/>
+      <c r="J50" s="51"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" s="18">
         <v>11</v>
       </c>
@@ -5330,50 +5504,70 @@
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H51" s="29"/>
+      <c r="I51" s="83"/>
+      <c r="J51" s="51"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" s="4">
         <v>12</v>
       </c>
-      <c r="C52" s="69" t="s">
+      <c r="C52" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D52" s="17"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H52" s="28"/>
+      <c r="I52" s="78"/>
+      <c r="J52" s="51"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B53" s="4">
         <v>13</v>
       </c>
-      <c r="C53" s="70"/>
+      <c r="C53" s="64"/>
       <c r="D53" s="17"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H53" s="28"/>
+      <c r="I53" s="78"/>
+      <c r="J53" s="51"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" s="4">
         <v>14</v>
       </c>
-      <c r="C54" s="70"/>
+      <c r="C54" s="64"/>
       <c r="D54" s="17"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H54" s="28"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="51"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B55" s="4">
         <v>15</v>
       </c>
-      <c r="C55" s="71"/>
+      <c r="C55" s="65"/>
       <c r="D55" s="17"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H55" s="28"/>
+      <c r="I55" s="51"/>
+      <c r="J55" s="51"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H56" s="51"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="51"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B58" s="4" t="s">
         <v>0</v>
       </c>
@@ -5383,99 +5577,107 @@
       <c r="D58" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="74" t="s">
+      <c r="E58" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="75"/>
-      <c r="G58" s="73" t="s">
+      <c r="F58" s="70"/>
+      <c r="G58" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="H58" s="73"/>
+      <c r="H58" s="67"/>
       <c r="I58" s="33" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J58" s="33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59" s="4">
         <v>0</v>
       </c>
-      <c r="C59" s="64" t="s">
+      <c r="C59" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="65" t="s">
+      <c r="D59" s="59" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="17"/>
       <c r="F59" s="17"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="39" t="s">
+      <c r="I59" s="38" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B60" s="4">
         <v>1</v>
       </c>
-      <c r="C60" s="64"/>
-      <c r="D60" s="65"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="59"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="39" t="s">
+      <c r="I60" s="38" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61" s="4">
         <v>2</v>
       </c>
-      <c r="C61" s="64"/>
-      <c r="D61" s="65"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="59"/>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="39" t="s">
+      <c r="I61" s="38" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B62" s="4">
         <v>3</v>
       </c>
-      <c r="C62" s="64"/>
-      <c r="D62" s="65"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="59"/>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="39" t="s">
+      <c r="I62" s="38" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B63" s="4">
         <v>4</v>
       </c>
-      <c r="C63" s="64"/>
+      <c r="C63" s="58"/>
       <c r="D63" s="16"/>
       <c r="E63" s="17"/>
       <c r="F63" s="17"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="39" t="s">
+      <c r="I63" s="38" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64" s="4">
         <v>5</v>
       </c>
-      <c r="C64" s="64"/>
+      <c r="C64" s="58"/>
       <c r="D64" s="17"/>
-      <c r="E64" s="53" t="s">
+      <c r="E64" s="71" t="s">
         <v>4</v>
       </c>
       <c r="F64" s="23" t="s">
@@ -5483,125 +5685,137 @@
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="39" t="s">
+      <c r="I64" s="38" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B65" s="4">
         <v>6</v>
       </c>
-      <c r="C65" s="64"/>
+      <c r="C65" s="58"/>
       <c r="D65" s="17"/>
-      <c r="E65" s="54"/>
+      <c r="E65" s="72"/>
       <c r="F65" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G65" s="58" t="s">
+      <c r="G65" s="75" t="s">
         <v>24</v>
       </c>
       <c r="H65" s="24" t="s">
         <v>26</v>
       </c>
       <c r="I65" s="1"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J65" s="85" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B66" s="4">
         <v>7</v>
       </c>
-      <c r="C66" s="64"/>
+      <c r="C66" s="58"/>
       <c r="D66" s="17"/>
-      <c r="E66" s="54"/>
+      <c r="E66" s="72"/>
       <c r="F66" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G66" s="59"/>
+      <c r="G66" s="76"/>
       <c r="H66" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I66" s="1"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J66" s="85" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B67" s="4">
         <v>8</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
-      <c r="E67" s="54"/>
+      <c r="E67" s="72"/>
       <c r="F67" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G67" s="59"/>
+      <c r="G67" s="76"/>
       <c r="H67" s="24" t="s">
         <v>28</v>
       </c>
       <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B68" s="4">
         <v>9</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
-      <c r="E68" s="54"/>
+      <c r="E68" s="72"/>
       <c r="F68" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G68" s="59"/>
+      <c r="G68" s="76"/>
       <c r="H68" s="24" t="s">
         <v>32</v>
       </c>
       <c r="I68" s="1"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B69" s="4">
         <v>10</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
-      <c r="E69" s="54"/>
+      <c r="E69" s="72"/>
       <c r="F69" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="59"/>
+      <c r="G69" s="76"/>
       <c r="H69" s="24" t="s">
         <v>31</v>
       </c>
       <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B70" s="4">
         <v>11</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
-      <c r="E70" s="54"/>
+      <c r="E70" s="72"/>
       <c r="F70" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="59"/>
+      <c r="G70" s="76"/>
       <c r="H70" s="24" t="s">
         <v>30</v>
       </c>
       <c r="I70" s="1"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B71" s="4">
         <v>12</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
-      <c r="E71" s="54"/>
+      <c r="E71" s="72"/>
       <c r="F71" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G71" s="60"/>
+      <c r="G71" s="77"/>
       <c r="H71" s="24" t="s">
         <v>29</v>
       </c>
       <c r="I71" s="1"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>42</v>
       </c>
@@ -5615,8 +5829,9 @@
       <c r="G72" s="29"/>
       <c r="H72" s="28"/>
       <c r="I72" s="1"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B73" s="15">
         <v>14</v>
       </c>
@@ -5627,8 +5842,9 @@
       <c r="G73" s="14"/>
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B74" s="15">
         <v>15</v>
       </c>
@@ -5639,19 +5855,25 @@
       <c r="G74" s="14"/>
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J74" s="1"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B77" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B78" s="4">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="K13:O13"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="G65:G71"/>
+    <mergeCell ref="G58:H58"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C59:C66"/>
     <mergeCell ref="D59:D62"/>
@@ -5664,11 +5886,6 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="E58:F58"/>
     <mergeCell ref="E64:E71"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="G65:G71"/>
-    <mergeCell ref="G58:H58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
UART complete, WWDG, IWDG, state_machine lib and code from post 3
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="157">
   <si>
     <t>Port C</t>
   </si>
@@ -497,6 +497,15 @@
   </si>
   <si>
     <t>UART2 RX (only 4 uart)</t>
+  </si>
+  <si>
+    <t>UART2 CK (synchronous)</t>
+  </si>
+  <si>
+    <t>UART1 CK (synchronous)</t>
+  </si>
+  <si>
+    <t>UART6 CK (synchronous)</t>
   </si>
 </sst>
 </file>
@@ -878,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1010,75 +1019,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1100,6 +1040,76 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4303,8 +4313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R52" zoomScale="224" workbookViewId="0">
-      <selection activeCell="F65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="104" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4314,19 +4324,19 @@
     <col min="7" max="7" width="17.109375" customWidth="1"/>
     <col min="8" max="8" width="20.88671875" customWidth="1"/>
     <col min="9" max="9" width="15.109375" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" customWidth="1"/>
+    <col min="10" max="10" width="23.109375" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="8.44140625" customWidth="1"/>
     <col min="13" max="14" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="57"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="73"/>
       <c r="F1" s="21"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4546,13 +4556,13 @@
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
-      <c r="K13" s="73" t="s">
+      <c r="K13" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="73"/>
-      <c r="M13" s="73"/>
-      <c r="N13" s="73"/>
-      <c r="O13" s="73"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="65"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
@@ -4578,10 +4588,10 @@
       <c r="M14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N14" s="68" t="s">
+      <c r="N14" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="O14" s="68"/>
+      <c r="O14" s="64"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="11"/>
@@ -4690,20 +4700,20 @@
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="68" t="s">
+      <c r="D20" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="68"/>
+      <c r="E20" s="64"/>
       <c r="F20" s="30" t="s">
         <v>77</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="H20" s="84" t="s">
+      <c r="H20" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="79"/>
+      <c r="I20" s="56"/>
       <c r="J20" s="51"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
@@ -4751,11 +4761,11 @@
       <c r="L22" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="N22" s="74" t="s">
+      <c r="N22" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="O22" s="74"/>
-      <c r="P22" s="74"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
@@ -4766,11 +4776,11 @@
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="85" t="s">
+      <c r="H23" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="I23" s="78"/>
-      <c r="J23" s="80"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="57"/>
       <c r="K23" s="32" t="s">
         <v>46</v>
       </c>
@@ -4796,10 +4806,10 @@
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="46"/>
-      <c r="H24" s="86" t="s">
+      <c r="H24" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="I24" s="81"/>
+      <c r="I24" s="58"/>
       <c r="J24" s="51"/>
       <c r="K24" s="15" t="s">
         <v>47</v>
@@ -4824,10 +4834,10 @@
       <c r="B25" s="3">
         <v>4</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="62" t="s">
+      <c r="D25" s="78" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="25" t="s">
@@ -4837,8 +4847,10 @@
         <v>81</v>
       </c>
       <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="78"/>
+      <c r="H25" s="87" t="s">
+        <v>154</v>
+      </c>
+      <c r="I25" s="55"/>
       <c r="J25" s="51"/>
       <c r="K25" s="15" t="s">
         <v>48</v>
@@ -4866,8 +4878,8 @@
       <c r="B26" s="35">
         <v>5</v>
       </c>
-      <c r="C26" s="60"/>
-      <c r="D26" s="62"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="78"/>
       <c r="E26" s="25" t="s">
         <v>35</v>
       </c>
@@ -4876,7 +4888,7 @@
       </c>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
-      <c r="I26" s="78"/>
+      <c r="I26" s="55"/>
       <c r="J26" s="51"/>
       <c r="K26" s="32" t="s">
         <v>49</v>
@@ -4898,8 +4910,8 @@
       <c r="B27" s="3">
         <v>6</v>
       </c>
-      <c r="C27" s="60"/>
-      <c r="D27" s="62"/>
+      <c r="C27" s="76"/>
+      <c r="D27" s="78"/>
       <c r="E27" s="25" t="s">
         <v>36</v>
       </c>
@@ -4908,7 +4920,7 @@
       </c>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
-      <c r="I27" s="78"/>
+      <c r="I27" s="55"/>
       <c r="J27" s="51"/>
       <c r="K27" s="32" t="s">
         <v>50</v>
@@ -4930,8 +4942,8 @@
       <c r="B28" s="3">
         <v>7</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="62"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="78"/>
       <c r="E28" s="25" t="s">
         <v>37</v>
       </c>
@@ -4940,7 +4952,7 @@
       </c>
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
-      <c r="I28" s="78"/>
+      <c r="I28" s="55"/>
       <c r="J28" s="51"/>
       <c r="K28" s="32" t="s">
         <v>51</v>
@@ -4962,17 +4974,19 @@
       <c r="B29" s="3">
         <v>8</v>
       </c>
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="62"/>
+      <c r="D29" s="78"/>
       <c r="E29" s="25" t="s">
         <v>38</v>
       </c>
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="78"/>
+      <c r="H29" s="87" t="s">
+        <v>155</v>
+      </c>
+      <c r="I29" s="55"/>
       <c r="J29" s="51"/>
       <c r="K29" s="32" t="s">
         <v>52</v>
@@ -4994,15 +5008,15 @@
       <c r="B30" s="3">
         <v>9</v>
       </c>
-      <c r="C30" s="61"/>
-      <c r="D30" s="62"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="78"/>
       <c r="E30" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
-      <c r="I30" s="78"/>
+      <c r="I30" s="55"/>
       <c r="J30" s="51"/>
       <c r="K30" s="32" t="s">
         <v>53</v>
@@ -5024,15 +5038,15 @@
       <c r="B31" s="3">
         <v>10</v>
       </c>
-      <c r="C31" s="61"/>
-      <c r="D31" s="62"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="78"/>
       <c r="E31" s="25" t="s">
         <v>40</v>
       </c>
       <c r="F31" s="36"/>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
-      <c r="I31" s="78"/>
+      <c r="I31" s="55"/>
       <c r="J31" s="51"/>
       <c r="K31" s="32" t="s">
         <v>54</v>
@@ -5054,15 +5068,15 @@
       <c r="B32" s="3">
         <v>11</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="78"/>
       <c r="E32" s="25" t="s">
         <v>41</v>
       </c>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
-      <c r="I32" s="78"/>
+      <c r="I32" s="55"/>
       <c r="J32" s="51"/>
       <c r="K32" s="32" t="s">
         <v>55</v>
@@ -5090,7 +5104,7 @@
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
-      <c r="I33" s="78"/>
+      <c r="I33" s="55"/>
       <c r="J33" s="51"/>
       <c r="K33" s="32" t="s">
         <v>56</v>
@@ -5118,7 +5132,7 @@
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="28"/>
-      <c r="I34" s="78"/>
+      <c r="I34" s="55"/>
       <c r="J34" s="51"/>
       <c r="K34" s="32" t="s">
         <v>57</v>
@@ -5146,7 +5160,7 @@
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
       <c r="H35" s="28"/>
-      <c r="I35" s="78"/>
+      <c r="I35" s="55"/>
       <c r="J35" s="51"/>
       <c r="K35" s="32" t="s">
         <v>58</v>
@@ -5174,7 +5188,7 @@
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
-      <c r="I36" s="78"/>
+      <c r="I36" s="55"/>
       <c r="J36" s="51"/>
       <c r="K36" s="32" t="s">
         <v>59</v>
@@ -5233,10 +5247,10 @@
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="67" t="s">
+      <c r="D39" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="E39" s="67"/>
+      <c r="E39" s="70"/>
       <c r="F39" s="32" t="s">
         <v>77</v>
       </c>
@@ -5246,7 +5260,7 @@
       <c r="H39" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="I39" s="82"/>
+      <c r="I39" s="59"/>
       <c r="J39" s="51"/>
       <c r="N39" s="40" t="s">
         <v>124</v>
@@ -5272,7 +5286,7 @@
         <v>131</v>
       </c>
       <c r="H40" s="28"/>
-      <c r="I40" s="78"/>
+      <c r="I40" s="55"/>
       <c r="J40" s="51"/>
       <c r="N40" s="43" t="s">
         <v>125</v>
@@ -5298,7 +5312,7 @@
         <v>132</v>
       </c>
       <c r="H41" s="28"/>
-      <c r="I41" s="78"/>
+      <c r="I41" s="55"/>
       <c r="J41" s="51"/>
       <c r="N41" s="43" t="s">
         <v>126</v>
@@ -5320,7 +5334,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="28"/>
-      <c r="I42" s="78"/>
+      <c r="I42" s="55"/>
       <c r="J42" s="51"/>
       <c r="N42" s="43" t="s">
         <v>127</v>
@@ -5342,7 +5356,7 @@
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
       <c r="H43" s="33"/>
-      <c r="I43" s="82"/>
+      <c r="I43" s="59"/>
       <c r="J43" s="51"/>
       <c r="N43" s="43" t="s">
         <v>128</v>
@@ -5359,7 +5373,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="4"/>
-      <c r="D44" s="66" t="s">
+      <c r="D44" s="82" t="s">
         <v>24</v>
       </c>
       <c r="E44" s="26" t="s">
@@ -5370,7 +5384,7 @@
         <v>133</v>
       </c>
       <c r="H44" s="28"/>
-      <c r="I44" s="78"/>
+      <c r="I44" s="55"/>
       <c r="J44" s="51"/>
       <c r="N44" s="43" t="s">
         <v>129</v>
@@ -5387,7 +5401,7 @@
         <v>5</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="66"/>
+      <c r="D45" s="82"/>
       <c r="E45" s="26" t="s">
         <v>27</v>
       </c>
@@ -5396,7 +5410,7 @@
         <v>134</v>
       </c>
       <c r="H45" s="28"/>
-      <c r="I45" s="78"/>
+      <c r="I45" s="55"/>
       <c r="J45" s="51"/>
       <c r="N45" s="43" t="s">
         <v>130</v>
@@ -5413,7 +5427,7 @@
         <v>6</v>
       </c>
       <c r="C46" s="4"/>
-      <c r="D46" s="66"/>
+      <c r="D46" s="82"/>
       <c r="E46" s="26" t="s">
         <v>28</v>
       </c>
@@ -5421,10 +5435,10 @@
       <c r="G46" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="H46" s="85" t="s">
+      <c r="H46" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="I46" s="78"/>
+      <c r="I46" s="55"/>
       <c r="J46" s="51"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.3">
@@ -5432,7 +5446,7 @@
         <v>7</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="66"/>
+      <c r="D47" s="82"/>
       <c r="E47" s="26" t="s">
         <v>32</v>
       </c>
@@ -5440,10 +5454,10 @@
       <c r="G47" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="H47" s="85" t="s">
+      <c r="H47" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="I47" s="78"/>
+      <c r="I47" s="55"/>
       <c r="J47" s="51"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.3">
@@ -5451,7 +5465,7 @@
         <v>8</v>
       </c>
       <c r="C48" s="4"/>
-      <c r="D48" s="66"/>
+      <c r="D48" s="82"/>
       <c r="E48" s="26" t="s">
         <v>31</v>
       </c>
@@ -5460,7 +5474,7 @@
         <v>137</v>
       </c>
       <c r="H48" s="28"/>
-      <c r="I48" s="78"/>
+      <c r="I48" s="55"/>
       <c r="J48" s="51"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
@@ -5468,7 +5482,7 @@
         <v>9</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="66"/>
+      <c r="D49" s="82"/>
       <c r="E49" s="26" t="s">
         <v>30</v>
       </c>
@@ -5477,7 +5491,7 @@
         <v>138</v>
       </c>
       <c r="H49" s="28"/>
-      <c r="I49" s="78"/>
+      <c r="I49" s="55"/>
       <c r="J49" s="51"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
@@ -5485,14 +5499,14 @@
         <v>10</v>
       </c>
       <c r="C50" s="4"/>
-      <c r="D50" s="66"/>
+      <c r="D50" s="82"/>
       <c r="E50" s="26" t="s">
         <v>29</v>
       </c>
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
-      <c r="I50" s="78"/>
+      <c r="I50" s="55"/>
       <c r="J50" s="51"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
@@ -5505,14 +5519,14 @@
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
       <c r="H51" s="29"/>
-      <c r="I51" s="83"/>
+      <c r="I51" s="60"/>
       <c r="J51" s="51"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" s="4">
         <v>12</v>
       </c>
-      <c r="C52" s="63" t="s">
+      <c r="C52" s="79" t="s">
         <v>12</v>
       </c>
       <c r="D52" s="17"/>
@@ -5520,27 +5534,27 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="28"/>
-      <c r="I52" s="78"/>
+      <c r="I52" s="55"/>
       <c r="J52" s="51"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B53" s="4">
         <v>13</v>
       </c>
-      <c r="C53" s="64"/>
+      <c r="C53" s="80"/>
       <c r="D53" s="17"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="28"/>
-      <c r="I53" s="78"/>
+      <c r="I53" s="55"/>
       <c r="J53" s="51"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" s="4">
         <v>14</v>
       </c>
-      <c r="C54" s="64"/>
+      <c r="C54" s="80"/>
       <c r="D54" s="17"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -5553,7 +5567,7 @@
       <c r="B55" s="4">
         <v>15</v>
       </c>
-      <c r="C55" s="65"/>
+      <c r="C55" s="81"/>
       <c r="D55" s="17"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -5577,14 +5591,14 @@
       <c r="D58" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="69" t="s">
+      <c r="E58" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="70"/>
-      <c r="G58" s="67" t="s">
+      <c r="F58" s="84"/>
+      <c r="G58" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="H58" s="67"/>
+      <c r="H58" s="70"/>
       <c r="I58" s="33" t="s">
         <v>78</v>
       </c>
@@ -5596,10 +5610,10 @@
       <c r="B59" s="4">
         <v>0</v>
       </c>
-      <c r="C59" s="58" t="s">
+      <c r="C59" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="59" t="s">
+      <c r="D59" s="75" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="17"/>
@@ -5615,8 +5629,8 @@
       <c r="B60" s="4">
         <v>1</v>
       </c>
-      <c r="C60" s="58"/>
-      <c r="D60" s="59"/>
+      <c r="C60" s="74"/>
+      <c r="D60" s="75"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
       <c r="G60" s="1"/>
@@ -5630,8 +5644,8 @@
       <c r="B61" s="4">
         <v>2</v>
       </c>
-      <c r="C61" s="58"/>
-      <c r="D61" s="59"/>
+      <c r="C61" s="74"/>
+      <c r="D61" s="75"/>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
       <c r="G61" s="1"/>
@@ -5645,8 +5659,8 @@
       <c r="B62" s="4">
         <v>3</v>
       </c>
-      <c r="C62" s="58"/>
-      <c r="D62" s="59"/>
+      <c r="C62" s="74"/>
+      <c r="D62" s="75"/>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
       <c r="G62" s="1"/>
@@ -5660,7 +5674,7 @@
       <c r="B63" s="4">
         <v>4</v>
       </c>
-      <c r="C63" s="58"/>
+      <c r="C63" s="74"/>
       <c r="D63" s="16"/>
       <c r="E63" s="17"/>
       <c r="F63" s="17"/>
@@ -5675,9 +5689,9 @@
       <c r="B64" s="4">
         <v>5</v>
       </c>
-      <c r="C64" s="58"/>
+      <c r="C64" s="74"/>
       <c r="D64" s="17"/>
-      <c r="E64" s="71" t="s">
+      <c r="E64" s="85" t="s">
         <v>4</v>
       </c>
       <c r="F64" s="23" t="s">
@@ -5694,20 +5708,20 @@
       <c r="B65" s="4">
         <v>6</v>
       </c>
-      <c r="C65" s="58"/>
+      <c r="C65" s="74"/>
       <c r="D65" s="17"/>
-      <c r="E65" s="72"/>
+      <c r="E65" s="86"/>
       <c r="F65" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G65" s="75" t="s">
+      <c r="G65" s="67" t="s">
         <v>24</v>
       </c>
       <c r="H65" s="24" t="s">
         <v>26</v>
       </c>
       <c r="I65" s="1"/>
-      <c r="J65" s="85" t="s">
+      <c r="J65" s="62" t="s">
         <v>148</v>
       </c>
     </row>
@@ -5715,18 +5729,18 @@
       <c r="B66" s="4">
         <v>7</v>
       </c>
-      <c r="C66" s="58"/>
+      <c r="C66" s="74"/>
       <c r="D66" s="17"/>
-      <c r="E66" s="72"/>
+      <c r="E66" s="86"/>
       <c r="F66" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G66" s="76"/>
+      <c r="G66" s="68"/>
       <c r="H66" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I66" s="1"/>
-      <c r="J66" s="85" t="s">
+      <c r="J66" s="62" t="s">
         <v>151</v>
       </c>
     </row>
@@ -5736,16 +5750,18 @@
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
-      <c r="E67" s="72"/>
+      <c r="E67" s="86"/>
       <c r="F67" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G67" s="76"/>
+      <c r="G67" s="68"/>
       <c r="H67" s="24" t="s">
         <v>28</v>
       </c>
       <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
+      <c r="J67" s="87" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B68" s="4">
@@ -5753,11 +5769,11 @@
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
-      <c r="E68" s="72"/>
+      <c r="E68" s="86"/>
       <c r="F68" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G68" s="76"/>
+      <c r="G68" s="68"/>
       <c r="H68" s="24" t="s">
         <v>32</v>
       </c>
@@ -5770,11 +5786,11 @@
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
-      <c r="E69" s="72"/>
+      <c r="E69" s="86"/>
       <c r="F69" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="G69" s="76"/>
+      <c r="G69" s="68"/>
       <c r="H69" s="24" t="s">
         <v>31</v>
       </c>
@@ -5787,11 +5803,11 @@
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
-      <c r="E70" s="72"/>
+      <c r="E70" s="86"/>
       <c r="F70" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="76"/>
+      <c r="G70" s="68"/>
       <c r="H70" s="24" t="s">
         <v>30</v>
       </c>
@@ -5804,11 +5820,11 @@
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
-      <c r="E71" s="72"/>
+      <c r="E71" s="86"/>
       <c r="F71" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G71" s="77"/>
+      <c r="G71" s="69"/>
       <c r="H71" s="24" t="s">
         <v>29</v>
       </c>
@@ -5869,11 +5885,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="K13:O13"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="G65:G71"/>
-    <mergeCell ref="G58:H58"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C59:C66"/>
     <mergeCell ref="D59:D62"/>
@@ -5886,6 +5897,11 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="E58:F58"/>
     <mergeCell ref="E64:E71"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="K13:O13"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="G65:G71"/>
+    <mergeCell ref="G58:H58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
iniciamos las librerias de i2c, agregamos a gpios la funcion de output type de open drain y push pull, configuramos en gpio output que sea push pull al igual que el tx en uart y en salidas pwm, cambiamos el nombre a funciones de uart, agregamos lib para sensor sht20, terminamos funciones deinit para uart
</commit_message>
<xml_diff>
--- a/documentation/pines y puertos disponibles.xlsx
+++ b/documentation/pines y puertos disponibles.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="161">
   <si>
     <t>Port C</t>
   </si>
@@ -50,33 +50,15 @@
     <t>4x4 teclado</t>
   </si>
   <si>
-    <t>Puerto A</t>
-  </si>
-  <si>
-    <t>Funcion 1</t>
-  </si>
-  <si>
-    <t>funcion 2</t>
-  </si>
-  <si>
     <t>Motor 4bits</t>
   </si>
   <si>
-    <t>funcion 1</t>
-  </si>
-  <si>
-    <t>funcion 3</t>
-  </si>
-  <si>
     <t>motor 8 bit</t>
   </si>
   <si>
     <t>motor 4 bits</t>
   </si>
   <si>
-    <t>Pines y puertos disponibles</t>
-  </si>
-  <si>
     <t>TIMERS</t>
   </si>
   <si>
@@ -108,9 +90,6 @@
   </si>
   <si>
     <t>LCD</t>
-  </si>
-  <si>
-    <t>funcion 4</t>
   </si>
   <si>
     <t>RS</t>
@@ -493,12 +472,6 @@
     <t>UART6 RX</t>
   </si>
   <si>
-    <t>UART2 TX (only 4 uart)</t>
-  </si>
-  <si>
-    <t>UART2 RX (only 4 uart)</t>
-  </si>
-  <si>
     <t>UART2 CK (synchronous)</t>
   </si>
   <si>
@@ -506,13 +479,52 @@
   </si>
   <si>
     <t>UART6 CK (synchronous)</t>
+  </si>
+  <si>
+    <t>I2C1_SCL</t>
+  </si>
+  <si>
+    <t>I2C1_SDA</t>
+  </si>
+  <si>
+    <t>I2C3_SDA</t>
+  </si>
+  <si>
+    <t>Function 7</t>
+  </si>
+  <si>
+    <t>I2C3_SCL</t>
+  </si>
+  <si>
+    <t>Function 2</t>
+  </si>
+  <si>
+    <t>Function 1</t>
+  </si>
+  <si>
+    <t>PINS and PORTS availables</t>
+  </si>
+  <si>
+    <t>Not connected</t>
+  </si>
+  <si>
+    <t>use SWO</t>
+  </si>
+  <si>
+    <t>Only for uart</t>
+  </si>
+  <si>
+    <t>UART2 TX (only for uart)</t>
+  </si>
+  <si>
+    <t>UART2 RX (only for uart)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,8 +548,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +684,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -699,21 +725,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -765,56 +776,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -883,11 +844,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -901,22 +931,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -941,7 +965,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -951,7 +975,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1012,25 +1036,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1043,6 +1056,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1052,22 +1088,25 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1088,28 +1127,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,7 +1173,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>780728</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>51982</xdr:rowOff>
@@ -1440,7 +1475,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>666901</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>140488</xdr:rowOff>
@@ -1705,7 +1740,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>32</xdr:col>
+      <xdr:col>36</xdr:col>
       <xdr:colOff>284964</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>90912</xdr:rowOff>
@@ -1901,7 +1936,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>554790</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>160422</xdr:rowOff>
@@ -2124,14 +2159,14 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>456562</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>47510</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>749504</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>749505</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>82280</xdr:rowOff>
     </xdr:to>
@@ -2162,7 +2197,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>12225</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>62712</xdr:rowOff>
@@ -2519,7 +2554,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>390071</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>165257</xdr:rowOff>
@@ -2728,7 +2763,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>682882</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>90872</xdr:rowOff>
@@ -3099,7 +3134,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>756478</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>101364</xdr:rowOff>
@@ -3463,7 +3498,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>73124</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>4496</xdr:rowOff>
@@ -3820,7 +3855,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>755453</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>44726</xdr:rowOff>
@@ -3889,7 +3924,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>719010</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>37075</xdr:rowOff>
@@ -3958,13 +3993,13 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>194553</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>129702</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>583175</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>4702</xdr:rowOff>
@@ -4311,10 +4346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:U78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="104" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4324,1007 +4359,1111 @@
     <col min="7" max="7" width="17.109375" customWidth="1"/>
     <col min="8" max="8" width="20.88671875" customWidth="1"/>
     <col min="9" max="9" width="15.109375" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="14" width="12.6640625" customWidth="1"/>
+    <col min="10" max="14" width="23.109375" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="16" max="16" width="8.44140625" customWidth="1"/>
+    <col min="17" max="18" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="71" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="21"/>
+    <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="76" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="11">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="9">
         <v>0</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="9">
         <v>0</v>
       </c>
       <c r="D3" s="7">
         <v>0</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>2</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="11">
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="9">
         <v>1</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="11">
+      <c r="E4" s="9"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B5" s="9">
         <v>4</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>2</v>
       </c>
       <c r="D5" s="7">
         <v>2</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="11">
+      <c r="E5" s="9"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="9">
         <v>5</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>4</v>
       </c>
       <c r="D6" s="7">
         <v>3</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="11">
+      <c r="E6" s="9"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B7" s="9">
         <v>6</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>5</v>
       </c>
       <c r="D7" s="7">
         <v>4</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="11">
+      <c r="E7" s="9"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B8" s="9">
         <v>7</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>6</v>
       </c>
       <c r="D8" s="7">
         <v>5</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="11">
+      <c r="E8" s="9"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="9">
         <v>8</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>7</v>
       </c>
       <c r="D9" s="7">
         <v>6</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="11">
+      <c r="E9" s="9"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B10" s="9">
         <v>9</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>8</v>
       </c>
       <c r="D10" s="7">
         <v>7</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="11">
+      <c r="E10" s="9"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B11" s="9">
         <v>10</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="9">
         <v>9</v>
       </c>
       <c r="D11" s="7">
         <v>8</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="11">
+      <c r="E11" s="9"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B12" s="9">
         <v>11</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="9">
         <v>10</v>
       </c>
       <c r="D12" s="7">
         <v>9</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="11">
+      <c r="E12" s="9"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="9">
         <v>12</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="9">
         <v>12</v>
       </c>
       <c r="D13" s="7">
         <v>10</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="K13" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="65"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="65"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="11">
+      <c r="E13" s="9"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="O13" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="69"/>
+      <c r="R13" s="69"/>
+      <c r="S13" s="69"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B14" s="9">
         <v>15</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="9">
         <v>13</v>
       </c>
       <c r="D14" s="7">
         <v>11</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="K14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N14" s="64" t="s">
-        <v>143</v>
-      </c>
-      <c r="O14" s="64"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11">
+      <c r="E14" s="9"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="O14" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="P14" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="R14" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="S14" s="68"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9">
         <v>14</v>
       </c>
       <c r="D15" s="7">
         <v>12</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="K15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L15" s="1">
+      <c r="E15" s="9"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="O15" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" s="58">
         <v>16</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12">
+      <c r="Q15" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="R15" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="S15" s="75"/>
+    </row>
+    <row r="16" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10">
         <v>15</v>
       </c>
       <c r="D16" s="8">
         <v>13</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="K16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" s="1">
+      <c r="E16" s="10"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="O16" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="58">
         <v>32</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q16" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="R16" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="S16" s="75"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
-      <c r="K17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="O17" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="P17" s="58">
         <v>16</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="K18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="1">
+      <c r="Q17" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="K19" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="1">
+      <c r="R17" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="S17" s="75"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="O18" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="P18" s="58">
         <v>16</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
-        <v>5</v>
+      <c r="Q18" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="R18" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="S18" s="75"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="O19" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="P19" s="58">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="R19" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="S19" s="75"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B20" s="57" t="s">
+        <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="64"/>
-      <c r="F20" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="H20" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20" s="56"/>
-      <c r="J20" s="51"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="D20" s="88" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="88"/>
+      <c r="F20" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="H20" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>0</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="L21" s="39" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F21" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="P21" s="37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>1</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" s="54" t="s">
-        <v>146</v>
-      </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="L22" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="N22" s="66" t="s">
-        <v>95</v>
-      </c>
-      <c r="O22" s="66"/>
-      <c r="P22" s="66"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B23" s="13">
+      <c r="F22" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="P22" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="R22" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="S22" s="70"/>
+      <c r="T22" s="70"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" s="11">
         <v>2</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="62" t="s">
-        <v>152</v>
-      </c>
-      <c r="I23" s="55"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="L23" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="N23" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="O23" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="P23" s="50" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B24" s="13">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="I23" s="26"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="P23" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="R23" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="S23" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="T23" s="48" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" s="11">
         <v>3</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="63" t="s">
-        <v>153</v>
-      </c>
-      <c r="I24" s="58"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L24" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="N24" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="O24" s="53" t="s">
-        <v>100</v>
-      </c>
-      <c r="P24" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="I24" s="62"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="P24" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R24" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="S24" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="T24" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="U24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <v>4</v>
       </c>
-      <c r="C25" s="76" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="78" t="s">
+      <c r="C25" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="87" t="s">
-        <v>154</v>
-      </c>
-      <c r="I25" s="55"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="L25" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="N25" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="O25" s="53" t="s">
-        <v>101</v>
-      </c>
-      <c r="P25" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="35">
+      <c r="E25" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="26"/>
+      <c r="H25" s="59" t="s">
+        <v>145</v>
+      </c>
+      <c r="I25" s="26"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="P25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R25" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="S25" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="T25" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="U25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="33">
         <v>5</v>
       </c>
-      <c r="C26" s="76"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="L26" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="N26" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="O26" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="P26" s="41" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C26" s="81"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="P26" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="R26" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="S26" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="T26" s="39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <v>6</v>
       </c>
-      <c r="C27" s="76"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="L27" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="N27" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="O27" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="P27" s="41" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C27" s="81"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="P27" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="R27" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="S27" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="T27" s="39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <v>7</v>
       </c>
-      <c r="C28" s="76"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="L28" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="N28" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="O28" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="P28" s="49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C28" s="81"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="P28" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="R28" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="S28" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="T28" s="47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <v>8</v>
       </c>
-      <c r="C29" s="77" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="78"/>
-      <c r="E29" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="87" t="s">
-        <v>155</v>
-      </c>
-      <c r="I29" s="55"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="L29" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="N29" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="O29" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="P29" s="49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C29" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="83"/>
+      <c r="E29" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="59" t="s">
+        <v>146</v>
+      </c>
+      <c r="I29" s="61" t="s">
+        <v>152</v>
+      </c>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="P29" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="R29" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="S29" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="T29" s="47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <v>9</v>
       </c>
-      <c r="C30" s="77"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="L30" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="N30" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="O30" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="P30" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C30" s="82"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="P30" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="R30" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="S30" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="T30" s="40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B31" s="3">
         <v>10</v>
       </c>
-      <c r="C31" s="77"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="36"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="L31" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="N31" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="O31" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="P31" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C31" s="82"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="34"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="P31" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="R31" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="S31" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="T31" s="40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B32" s="3">
         <v>11</v>
       </c>
-      <c r="C32" s="77"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="51"/>
-      <c r="K32" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="L32" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="N32" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="O32" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="P32" s="41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C32" s="82"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="P32" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="R32" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="S32" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="T32" s="39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B33" s="3">
         <v>12</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="32" t="s">
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="P33" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="R33" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="S33" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="T33" s="39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B34" s="11">
+        <v>13</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="P34" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="L33" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="N33" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="O33" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="P33" s="41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B34" s="13">
-        <v>13</v>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="32" t="s">
+      <c r="R34" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="S34" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="T34" s="39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B35" s="11">
+        <v>14</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="P35" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="L34" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="N34" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="O34" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="P34" s="41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B35" s="13">
-        <v>14</v>
-      </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="L35" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="N35" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="O35" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="P35" s="41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="R35" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="S35" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="T35" s="39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B36" s="3">
         <v>15</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="32" t="s">
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="P36" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="R36" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="S36" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="T36" s="39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="P37" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="L36" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="N36" s="40" t="s">
-        <v>121</v>
-      </c>
-      <c r="O36" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="P36" s="41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="H37" s="51"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="L37" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="N37" s="40" t="s">
-        <v>122</v>
-      </c>
-      <c r="O37" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="P37" s="41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="H38" s="51"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="51"/>
-      <c r="N38" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="O38" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="P38" s="41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="R37" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="S37" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="T37" s="39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="R38" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="S38" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="T38" s="39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B39" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="70"/>
-      <c r="F39" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="G39" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="H39" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="I39" s="59"/>
-      <c r="J39" s="51"/>
-      <c r="N39" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="O39" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="P39" s="41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="D39" s="68" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" s="68"/>
+      <c r="F39" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="H39" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I39" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="R39" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="S39" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="T39" s="39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B40" s="4">
         <v>0</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="G40" s="47" t="s">
-        <v>131</v>
-      </c>
-      <c r="H40" s="28"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="51"/>
-      <c r="N40" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="O40" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="P40" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F40" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G40" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="R40" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="S40" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="T40" s="40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B41" s="4">
         <v>1</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="G41" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="H41" s="28"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="51"/>
-      <c r="N41" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="O41" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="P41" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F41" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
+      <c r="R41" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="S41" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="T41" s="40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B42" s="4">
         <v>2</v>
       </c>
@@ -5333,558 +5472,700 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="28"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="51"/>
-      <c r="N42" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="O42" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="P42" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B43" s="15">
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49"/>
+      <c r="R42" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="S42" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="T42" s="40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" s="13">
         <v>3</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="59"/>
-      <c r="J43" s="51"/>
-      <c r="N43" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="O43" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="P43" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49"/>
+      <c r="R43" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="S43" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="T43" s="40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B44" s="4">
         <v>4</v>
       </c>
       <c r="C44" s="4"/>
-      <c r="D44" s="82" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="28"/>
-      <c r="G44" s="47" t="s">
+      <c r="D44" s="87" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="26"/>
+      <c r="G44" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
+      <c r="R44" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="S44" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="T44" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="H44" s="28"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="51"/>
-      <c r="N44" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="O44" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="P44" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B45" s="4">
         <v>5</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" s="28"/>
-      <c r="G45" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="H45" s="28"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="51"/>
-      <c r="N45" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="O45" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="P45" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D45" s="87"/>
+      <c r="E45" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="26"/>
+      <c r="G45" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="49"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="R45" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="S45" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="T45" s="40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B46" s="4">
         <v>6</v>
       </c>
       <c r="C46" s="4"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="F46" s="28"/>
-      <c r="G46" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="H46" s="62" t="s">
-        <v>147</v>
-      </c>
-      <c r="I46" s="55"/>
-      <c r="J46" s="51"/>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D46" s="87"/>
+      <c r="E46" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="26"/>
+      <c r="G46" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="H46" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="I46" s="26"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+      <c r="L46" s="49"/>
+      <c r="M46" s="49"/>
+      <c r="N46" s="49"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B47" s="4">
         <v>7</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F47" s="28"/>
-      <c r="G47" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="H47" s="62" t="s">
-        <v>149</v>
-      </c>
-      <c r="I47" s="55"/>
-      <c r="J47" s="51"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D47" s="87"/>
+      <c r="E47" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" s="26"/>
+      <c r="G47" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="H47" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="I47" s="26"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="49"/>
+      <c r="L47" s="49"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="49"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B48" s="4">
         <v>8</v>
       </c>
       <c r="C48" s="4"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="H48" s="28"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="51"/>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D48" s="87"/>
+      <c r="E48" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="26"/>
+      <c r="G48" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="H48" s="26"/>
+      <c r="I48" s="61" t="s">
+        <v>148</v>
+      </c>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="49"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="49"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B49" s="4">
         <v>9</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F49" s="28"/>
-      <c r="G49" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="H49" s="28"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="51"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D49" s="87"/>
+      <c r="E49" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49" s="26"/>
+      <c r="G49" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="H49" s="26"/>
+      <c r="I49" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="J49" s="49"/>
+      <c r="K49" s="49"/>
+      <c r="L49" s="49"/>
+      <c r="M49" s="49"/>
+      <c r="N49" s="49"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B50" s="4">
         <v>10</v>
       </c>
       <c r="C50" s="4"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="51"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B51" s="18">
+      <c r="D50" s="87"/>
+      <c r="E50" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="49"/>
+      <c r="N50" s="49"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="16">
         <v>11</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="60"/>
-      <c r="J51" s="51"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C51" s="17"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="27"/>
+      <c r="J51" s="49"/>
+      <c r="K51" s="49"/>
+      <c r="L51" s="49"/>
+      <c r="M51" s="49"/>
+      <c r="N51" s="49"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B52" s="4">
         <v>12</v>
       </c>
-      <c r="C52" s="79" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="17"/>
+      <c r="C52" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="15"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="55"/>
-      <c r="J52" s="51"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="49"/>
+      <c r="K52" s="49"/>
+      <c r="L52" s="49"/>
+      <c r="M52" s="49"/>
+      <c r="N52" s="49"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B53" s="4">
         <v>13</v>
       </c>
-      <c r="C53" s="80"/>
-      <c r="D53" s="17"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="15"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="28"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="51"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="49"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="49"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B54" s="4">
         <v>14</v>
       </c>
-      <c r="C54" s="80"/>
-      <c r="D54" s="17"/>
+      <c r="C54" s="85"/>
+      <c r="D54" s="15"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="51"/>
-      <c r="J54" s="51"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="49"/>
+      <c r="L54" s="49"/>
+      <c r="M54" s="49"/>
+      <c r="N54" s="49"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B55" s="4">
         <v>15</v>
       </c>
-      <c r="C55" s="81"/>
-      <c r="D55" s="17"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="15"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="51"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H56" s="51"/>
-      <c r="I56" s="51"/>
-      <c r="J56" s="51"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="49"/>
+      <c r="L55" s="49"/>
+      <c r="M55" s="49"/>
+      <c r="N55" s="49"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H56" s="49"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
+      <c r="L56" s="49"/>
+      <c r="M56" s="49"/>
+      <c r="N56" s="49"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B58" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>9</v>
+        <v>154</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="F58" s="84"/>
-      <c r="G58" s="70" t="s">
-        <v>25</v>
-      </c>
-      <c r="H58" s="70"/>
-      <c r="I58" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="J58" s="33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="E58" s="74" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="75"/>
+      <c r="G58" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="H58" s="68"/>
+      <c r="I58" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="J58" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="K58" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="L58" s="53"/>
+      <c r="M58" s="53"/>
+      <c r="N58" s="53"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B59" s="4">
         <v>0</v>
       </c>
-      <c r="C59" s="74" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
+      <c r="C59" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="38" t="s">
-        <v>87</v>
+      <c r="I59" s="36" t="s">
+        <v>80</v>
       </c>
       <c r="J59" s="1"/>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K59" s="1"/>
+      <c r="L59" s="60"/>
+      <c r="M59" s="60"/>
+      <c r="N59" s="60"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B60" s="4">
         <v>1</v>
       </c>
-      <c r="C60" s="74"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
+      <c r="C60" s="79"/>
+      <c r="D60" s="80"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="38" t="s">
-        <v>88</v>
+      <c r="I60" s="36" t="s">
+        <v>81</v>
       </c>
       <c r="J60" s="1"/>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K60" s="1"/>
+      <c r="L60" s="60"/>
+      <c r="M60" s="60"/>
+      <c r="N60" s="60"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B61" s="4">
         <v>2</v>
       </c>
-      <c r="C61" s="74"/>
-      <c r="D61" s="75"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
+      <c r="C61" s="79"/>
+      <c r="D61" s="80"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="38" t="s">
-        <v>89</v>
+      <c r="I61" s="36" t="s">
+        <v>82</v>
       </c>
       <c r="J61" s="1"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K61" s="1"/>
+      <c r="L61" s="60"/>
+      <c r="M61" s="60"/>
+      <c r="N61" s="60"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B62" s="4">
         <v>3</v>
       </c>
-      <c r="C62" s="74"/>
-      <c r="D62" s="75"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
+      <c r="C62" s="79"/>
+      <c r="D62" s="80"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="38" t="s">
-        <v>90</v>
+      <c r="I62" s="36" t="s">
+        <v>83</v>
       </c>
       <c r="J62" s="1"/>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K62" s="1"/>
+      <c r="L62" s="60"/>
+      <c r="M62" s="60"/>
+      <c r="N62" s="60"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B63" s="4">
         <v>4</v>
       </c>
-      <c r="C63" s="74"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
+      <c r="C63" s="79"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="38" t="s">
-        <v>91</v>
+      <c r="I63" s="36" t="s">
+        <v>84</v>
       </c>
       <c r="J63" s="1"/>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="K63" s="1"/>
+      <c r="L63" s="60"/>
+      <c r="M63" s="60"/>
+      <c r="N63" s="60"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B64" s="4">
         <v>5</v>
       </c>
-      <c r="C64" s="74"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="85" t="s">
+      <c r="C64" s="79"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="F64" s="23" t="s">
-        <v>34</v>
+      <c r="F64" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="38" t="s">
-        <v>92</v>
+      <c r="I64" s="36" t="s">
+        <v>85</v>
       </c>
       <c r="J64" s="1"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K64" s="26"/>
+      <c r="L64" s="50"/>
+      <c r="M64" s="50"/>
+      <c r="N64" s="50"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B65" s="4">
         <v>6</v>
       </c>
-      <c r="C65" s="74"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="86"/>
-      <c r="F65" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="G65" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="H65" s="24" t="s">
-        <v>26</v>
+      <c r="C65" s="79"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="90"/>
+      <c r="F65" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G65" s="71" t="s">
+        <v>18</v>
+      </c>
+      <c r="H65" s="22" t="s">
+        <v>19</v>
       </c>
       <c r="I65" s="1"/>
-      <c r="J65" s="62" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J65" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="K65" s="54"/>
+      <c r="L65" s="51"/>
+      <c r="M65" s="51"/>
+      <c r="N65" s="51"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B66" s="4">
         <v>7</v>
       </c>
-      <c r="C66" s="74"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="86"/>
-      <c r="F66" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G66" s="68"/>
-      <c r="H66" s="24" t="s">
-        <v>27</v>
+      <c r="C66" s="79"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="90"/>
+      <c r="F66" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" s="72"/>
+      <c r="H66" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="I66" s="1"/>
-      <c r="J66" s="62" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J66" s="55" t="s">
+        <v>144</v>
+      </c>
+      <c r="K66" s="54"/>
+      <c r="L66" s="51"/>
+      <c r="M66" s="51"/>
+      <c r="N66" s="51"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B67" s="4">
         <v>8</v>
       </c>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
-      <c r="E67" s="86"/>
-      <c r="F67" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G67" s="68"/>
-      <c r="H67" s="24" t="s">
-        <v>28</v>
+      <c r="E67" s="90"/>
+      <c r="F67" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="72"/>
+      <c r="H67" s="22" t="s">
+        <v>21</v>
       </c>
       <c r="I67" s="1"/>
-      <c r="J67" s="87" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J67" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="K67" s="26"/>
+      <c r="L67" s="50"/>
+      <c r="M67" s="50"/>
+      <c r="N67" s="50"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B68" s="4">
         <v>9</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
-      <c r="E68" s="86"/>
-      <c r="F68" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G68" s="68"/>
-      <c r="H68" s="24" t="s">
-        <v>32</v>
+      <c r="E68" s="90"/>
+      <c r="F68" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G68" s="72"/>
+      <c r="H68" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K68" s="61" t="s">
+        <v>150</v>
+      </c>
+      <c r="L68" s="50"/>
+      <c r="M68" s="50"/>
+      <c r="N68" s="50"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B69" s="4">
         <v>10</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
-      <c r="E69" s="86"/>
-      <c r="F69" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="G69" s="68"/>
-      <c r="H69" s="24" t="s">
-        <v>31</v>
+      <c r="E69" s="90"/>
+      <c r="F69" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" s="72"/>
+      <c r="H69" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K69" s="1"/>
+      <c r="L69" s="60"/>
+      <c r="M69" s="60"/>
+      <c r="N69" s="60"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B70" s="4">
         <v>11</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
-      <c r="E70" s="86"/>
-      <c r="F70" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="G70" s="68"/>
-      <c r="H70" s="24" t="s">
-        <v>30</v>
+      <c r="E70" s="90"/>
+      <c r="F70" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G70" s="72"/>
+      <c r="H70" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K70" s="1"/>
+      <c r="L70" s="60"/>
+      <c r="M70" s="60"/>
+      <c r="N70" s="60"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B71" s="4">
         <v>12</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
-      <c r="E71" s="86"/>
-      <c r="F71" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G71" s="69"/>
-      <c r="H71" s="24" t="s">
-        <v>29</v>
+      <c r="E71" s="90"/>
+      <c r="F71" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G71" s="73"/>
+      <c r="H71" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K71" s="1"/>
+      <c r="L71" s="60"/>
+      <c r="M71" s="60"/>
+      <c r="N71" s="60"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B72" s="31">
+        <v>35</v>
+      </c>
+      <c r="B72" s="29">
         <v>13</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
-      <c r="E72" s="27"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="29"/>
-      <c r="H72" s="28"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="26"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B73" s="15">
+      <c r="K72" s="1"/>
+      <c r="L72" s="60"/>
+      <c r="M72" s="60"/>
+      <c r="N72" s="60"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B73" s="13">
         <v>14</v>
       </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="15"/>
-      <c r="E73" s="15"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
       <c r="J73" s="1"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B74" s="15">
+      <c r="K73" s="1"/>
+      <c r="L73" s="60"/>
+      <c r="M73" s="60"/>
+      <c r="N73" s="60"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B74" s="13">
         <v>15</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="15"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
       <c r="J74" s="1"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K74" s="1"/>
+      <c r="L74" s="60"/>
+      <c r="M74" s="60"/>
+      <c r="N74" s="60"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B77" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B78" s="4">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="22">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C59:C66"/>
     <mergeCell ref="D59:D62"/>
@@ -5897,11 +6178,16 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="E58:F58"/>
     <mergeCell ref="E64:E71"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="K13:O13"/>
-    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="O13:S13"/>
+    <mergeCell ref="R22:T22"/>
     <mergeCell ref="G65:G71"/>
     <mergeCell ref="G58:H58"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>